<commit_message>
fix data, date, style
</commit_message>
<xml_diff>
--- a/work_doc_4.xlsx
+++ b/work_doc_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/MyProjects/script_for_receipts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{636AE084-0AA8-5441-86DF-0B5B2ABF4FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F8980C5A-965E-1245-94C8-8822DBCB5ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15840" tabRatio="779" activeTab="1" xr2:uid="{2706A050-E929-D447-803A-56A6BD4AC902}"/>
   </bookViews>
@@ -382,17 +382,11 @@
     <t>текст шапки</t>
   </si>
   <si>
-    <t>53/а</t>
-  </si>
-  <si>
     <t>смена
 счетчика</t>
   </si>
   <si>
     <t>Трактин В.В.</t>
-  </si>
-  <si>
-    <t>53/б</t>
   </si>
   <si>
     <t xml:space="preserve">Митрофанова И.В. </t>
@@ -408,6 +402,12 @@
   </si>
   <si>
     <t>БИК 044525411; Р/с 40703810824317000026; К/с 30101810145250000411</t>
+  </si>
+  <si>
+    <t>53-а</t>
+  </si>
+  <si>
+    <t>53-б</t>
   </si>
 </sst>
 </file>
@@ -1104,35 +1104,32 @@
     <xf numFmtId="17" fontId="20" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1152,9 +1149,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1167,23 +1161,17 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1193,6 +1181,18 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1512,10 +1512,10 @@
   <dimension ref="A1:BL162"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="AO14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="AO40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomRight" activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
@@ -1652,7 +1652,7 @@
         <v>2025-04-01</v>
       </c>
       <c r="AM1" s="117" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AN1" s="117"/>
       <c r="AO1" s="112" t="d">
@@ -7406,7 +7406,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="78" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43" s="32">
         <f t="shared" si="2"/>
@@ -7546,7 +7546,7 @@
         <v>23</v>
       </c>
       <c r="B44" s="80" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" s="32">
         <f t="shared" si="2"/>
@@ -11043,7 +11043,7 @@
         <v>38</v>
       </c>
       <c r="B69" s="78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C69" s="32">
         <f t="shared" si="4"/>
@@ -11060,7 +11060,7 @@
         <v>15802.54</v>
       </c>
       <c r="G69" s="71" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="H69" s="29">
         <v>16940.91</v>
@@ -11185,7 +11185,7 @@
         <v>38</v>
       </c>
       <c r="B70" s="80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C70" s="32">
         <f t="shared" si="4"/>
@@ -11198,7 +11198,7 @@
       <c r="E70" s="77"/>
       <c r="F70" s="84"/>
       <c r="G70" s="71" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="H70" s="29">
         <v>9688.8700000000008</v>
@@ -11340,7 +11340,7 @@
         <v>3236.91</v>
       </c>
       <c r="G71" s="71" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="H71" s="24">
         <v>0</v>
@@ -11478,7 +11478,7 @@
       <c r="E72" s="77"/>
       <c r="F72" s="84"/>
       <c r="G72" s="71" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="H72" s="24">
         <v>0</v>
@@ -12900,7 +12900,7 @@
         <v>45</v>
       </c>
       <c r="B82" s="78" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C82" s="32">
         <f t="shared" si="4"/>
@@ -13042,7 +13042,7 @@
         <v>45</v>
       </c>
       <c r="B83" s="80" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C83" s="32">
         <f t="shared" si="4"/>
@@ -13219,19 +13219,19 @@
     </row>
     <row r="94" spans="1:46">
       <c r="B94" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E94" s="54"/>
     </row>
     <row r="95" spans="1:46">
       <c r="B95" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E95" s="54"/>
     </row>
     <row r="96" spans="1:46">
       <c r="B96" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E96" s="54"/>
     </row>
@@ -13462,8 +13462,8 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:X114"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="190" zoomScaleNormal="115" zoomScaleSheetLayoutView="190" zoomScalePageLayoutView="108" workbookViewId="0">
-      <selection activeCell="V42" sqref="V42:V43"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A67" zoomScale="190" zoomScaleNormal="115" zoomScaleSheetLayoutView="190" zoomScalePageLayoutView="108" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="11"/>
@@ -13510,11 +13510,11 @@
       <c r="Q1" s="110"/>
       <c r="R1" s="110"/>
       <c r="S1" s="111"/>
-      <c r="T1" s="120" t="d">
+      <c r="T1" s="139" t="d">
         <f>Архив!B1</f>
         <v>2025-10-01</v>
       </c>
-      <c r="U1" s="120"/>
+      <c r="U1" s="139"/>
       <c r="V1" s="107"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1">
@@ -13654,43 +13654,43 @@
     </row>
     <row r="7" spans="1:24" s="1" customFormat="1" ht="21.75" customHeight="1">
       <c r="A7" s="20"/>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131" t="s">
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="131" t="s">
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="132"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="131" t="s">
+      <c r="K7" s="131"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="N7" s="132"/>
-      <c r="O7" s="133"/>
-      <c r="P7" s="131" t="s">
+      <c r="N7" s="131"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="Q7" s="132"/>
-      <c r="R7" s="133"/>
-      <c r="S7" s="123" t="s">
+      <c r="Q7" s="131"/>
+      <c r="R7" s="132"/>
+      <c r="S7" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="T7" s="135" t="s">
+      <c r="T7" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="U7" s="123" t="s">
+      <c r="U7" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="V7" s="123" t="s">
+      <c r="V7" s="137" t="s">
         <v>11</v>
       </c>
       <c r="W7" s="20"/>
@@ -13748,10 +13748,10 @@
       <c r="R8" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="S8" s="124"/>
-      <c r="T8" s="136"/>
-      <c r="U8" s="124"/>
-      <c r="V8" s="124"/>
+      <c r="S8" s="138"/>
+      <c r="T8" s="134"/>
+      <c r="U8" s="138"/>
+      <c r="V8" s="138"/>
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
     </row>
@@ -13824,15 +13824,15 @@
     </row>
     <row r="10" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A10" s="21"/>
-      <c r="B10" s="118">
+      <c r="B10" s="123">
         <f>Архив!A2</f>
         <v>1</v>
       </c>
-      <c r="C10" s="126">
+      <c r="C10" s="119">
         <f>Архив!G2</f>
         <v>21</v>
       </c>
-      <c r="D10" s="137" t="s">
+      <c r="D10" s="135" t="s">
         <v>57</v>
       </c>
       <c r="E10" s="12" t="s">
@@ -13887,19 +13887,19 @@
         <f t="shared" ref="R10:R41" si="3">IF(L10&lt;0,0,L10*O10)</f>
         <v>0</v>
       </c>
-      <c r="S10" s="122">
+      <c r="S10" s="121">
         <f>ROUND(SUM(P10:R11),2)</f>
         <v>30.59</v>
       </c>
-      <c r="T10" s="122">
+      <c r="T10" s="121">
         <f>Архив!E2</f>
         <v>-282.56999999999988</v>
       </c>
-      <c r="U10" s="122">
+      <c r="U10" s="121">
         <f>Архив!F2</f>
         <v>500</v>
       </c>
-      <c r="V10" s="122">
+      <c r="V10" s="121">
         <f>SUM(S10:T11)-U10</f>
         <v>-751.9799999999999</v>
       </c>
@@ -13908,11 +13908,11 @@
     </row>
     <row r="11" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A11" s="21"/>
-      <c r="B11" s="119" t="s">
+      <c r="B11" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="126"/>
-      <c r="D11" s="138" t="str">
+      <c r="C11" s="119"/>
+      <c r="D11" s="136" t="str">
         <f>D10</f>
         <v>Гаценко Н.Г.</v>
       </c>
@@ -13968,24 +13968,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S11" s="122"/>
-      <c r="T11" s="122"/>
-      <c r="U11" s="122"/>
-      <c r="V11" s="122"/>
+      <c r="S11" s="121"/>
+      <c r="T11" s="121"/>
+      <c r="U11" s="121"/>
+      <c r="V11" s="121"/>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
     <row r="12" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A12" s="21"/>
-      <c r="B12" s="118">
+      <c r="B12" s="123">
         <f>Архив!A4</f>
         <v>2</v>
       </c>
-      <c r="C12" s="126">
+      <c r="C12" s="119">
         <f>Архив!G4</f>
         <v>54</v>
       </c>
-      <c r="D12" s="134" t="s">
+      <c r="D12" s="122" t="s">
         <v>58</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -14044,11 +14044,11 @@
         <f>ROUND(SUM(P12:R13),2)</f>
         <v>0</v>
       </c>
-      <c r="T12" s="122">
+      <c r="T12" s="121">
         <f>Архив!E4</f>
         <v>0</v>
       </c>
-      <c r="U12" s="122">
+      <c r="U12" s="121">
         <f>Архив!F8</f>
         <v>0</v>
       </c>
@@ -14061,11 +14061,11 @@
     </row>
     <row r="13" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A13" s="21"/>
-      <c r="B13" s="119" t="s">
+      <c r="B13" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="126"/>
-      <c r="D13" s="134" t="str">
+      <c r="C13" s="119"/>
+      <c r="D13" s="122" t="str">
         <f>D12</f>
         <v>Дикарев А.А.</v>
       </c>
@@ -14122,23 +14122,23 @@
         <v>0</v>
       </c>
       <c r="S13" s="125"/>
-      <c r="T13" s="122"/>
-      <c r="U13" s="122"/>
+      <c r="T13" s="121"/>
+      <c r="U13" s="121"/>
       <c r="V13" s="125"/>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
     <row r="14" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A14" s="21"/>
-      <c r="B14" s="118">
+      <c r="B14" s="123">
         <f>Архив!A6</f>
         <v>3</v>
       </c>
-      <c r="C14" s="126">
+      <c r="C14" s="119">
         <f>Архив!G6</f>
         <v>51</v>
       </c>
-      <c r="D14" s="134" t="s">
+      <c r="D14" s="122" t="s">
         <v>59</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -14193,15 +14193,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S14" s="122">
+      <c r="S14" s="121">
         <f>ROUND(SUM(P14:R15),2)</f>
         <v>2184.7600000000002</v>
       </c>
-      <c r="T14" s="122">
+      <c r="T14" s="121">
         <f>Архив!E6</f>
         <v>8160.23</v>
       </c>
-      <c r="U14" s="122">
+      <c r="U14" s="121">
         <f>Архив!F6</f>
         <v>0</v>
       </c>
@@ -14214,11 +14214,11 @@
     </row>
     <row r="15" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A15" s="21"/>
-      <c r="B15" s="119" t="s">
+      <c r="B15" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="126"/>
-      <c r="D15" s="134" t="str">
+      <c r="C15" s="119"/>
+      <c r="D15" s="122" t="str">
         <f>D14</f>
         <v>Дмитриев А.В.</v>
       </c>
@@ -14274,24 +14274,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S15" s="122"/>
-      <c r="T15" s="122"/>
-      <c r="U15" s="122"/>
+      <c r="S15" s="121"/>
+      <c r="T15" s="121"/>
+      <c r="U15" s="121"/>
       <c r="V15" s="125"/>
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
     <row r="16" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A16" s="21"/>
-      <c r="B16" s="118">
+      <c r="B16" s="123">
         <f>Архив!A8</f>
         <v>4</v>
       </c>
-      <c r="C16" s="126">
+      <c r="C16" s="119">
         <f>Архив!G8</f>
         <v>35</v>
       </c>
-      <c r="D16" s="127" t="s">
+      <c r="D16" s="120" t="s">
         <v>60</v>
       </c>
       <c r="E16" s="12" t="s">
@@ -14346,19 +14346,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S16" s="122">
+      <c r="S16" s="121">
         <f>ROUND(SUM(P16:R17),2)</f>
         <v>1212.57</v>
       </c>
-      <c r="T16" s="122">
+      <c r="T16" s="121">
         <f>Архив!E8</f>
         <v>2391.64</v>
       </c>
-      <c r="U16" s="122">
+      <c r="U16" s="121">
         <f>Архив!F8</f>
         <v>0</v>
       </c>
-      <c r="V16" s="122">
+      <c r="V16" s="121">
         <f>SUM(S16:T17)-U16</f>
         <v>3604.21</v>
       </c>
@@ -14367,11 +14367,11 @@
     </row>
     <row r="17" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A17" s="21"/>
-      <c r="B17" s="119" t="s">
+      <c r="B17" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="126"/>
-      <c r="D17" s="127" t="str">
+      <c r="C17" s="119"/>
+      <c r="D17" s="120" t="str">
         <f>D16</f>
         <v>Егоров Е.Ю.</v>
       </c>
@@ -14427,24 +14427,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S17" s="122"/>
-      <c r="T17" s="122"/>
-      <c r="U17" s="122"/>
-      <c r="V17" s="122"/>
+      <c r="S17" s="121"/>
+      <c r="T17" s="121"/>
+      <c r="U17" s="121"/>
+      <c r="V17" s="121"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
     </row>
     <row r="18" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A18" s="21"/>
-      <c r="B18" s="118">
+      <c r="B18" s="123">
         <f>Архив!A10</f>
         <v>5</v>
       </c>
-      <c r="C18" s="126">
+      <c r="C18" s="119">
         <f>Архив!G10</f>
         <v>46</v>
       </c>
-      <c r="D18" s="127" t="s">
+      <c r="D18" s="120" t="s">
         <v>61</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -14499,19 +14499,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S18" s="122">
+      <c r="S18" s="121">
         <f>ROUND(SUM(P18:R19),2)</f>
         <v>153.97</v>
       </c>
-      <c r="T18" s="122">
+      <c r="T18" s="121">
         <f>Архив!E10</f>
         <v>-299.95</v>
       </c>
-      <c r="U18" s="122">
+      <c r="U18" s="121">
         <f>Архив!F10</f>
         <v>0</v>
       </c>
-      <c r="V18" s="122">
+      <c r="V18" s="121">
         <f>SUM(S18:T19)-U18</f>
         <v>-145.97999999999999</v>
       </c>
@@ -14520,11 +14520,11 @@
     </row>
     <row r="19" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A19" s="21"/>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="126"/>
-      <c r="D19" s="127" t="str">
+      <c r="C19" s="119"/>
+      <c r="D19" s="120" t="str">
         <f>D18</f>
         <v>Ефимов В.В.</v>
       </c>
@@ -14580,10 +14580,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S19" s="122"/>
-      <c r="T19" s="122"/>
-      <c r="U19" s="122"/>
-      <c r="V19" s="122"/>
+      <c r="S19" s="121"/>
+      <c r="T19" s="121"/>
+      <c r="U19" s="121"/>
+      <c r="V19" s="121"/>
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
@@ -14673,15 +14673,15 @@
     </row>
     <row r="21" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A21" s="21"/>
-      <c r="B21" s="140">
+      <c r="B21" s="118">
         <f>Архив!A13</f>
         <v>7</v>
       </c>
-      <c r="C21" s="126">
+      <c r="C21" s="119">
         <f>Архив!G13</f>
         <v>3</v>
       </c>
-      <c r="D21" s="127" t="s">
+      <c r="D21" s="120" t="s">
         <v>63</v>
       </c>
       <c r="E21" s="12" t="s">
@@ -14736,19 +14736,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S21" s="122">
+      <c r="S21" s="121">
         <f>ROUND(SUM(P21:R22),2)</f>
         <v>1427.21</v>
       </c>
-      <c r="T21" s="122">
+      <c r="T21" s="121">
         <f>Архив!E13</f>
         <v>1079.5599999999995</v>
       </c>
-      <c r="U21" s="122">
+      <c r="U21" s="121">
         <f>Архив!F13</f>
         <v>1081.4000000000001</v>
       </c>
-      <c r="V21" s="122">
+      <c r="V21" s="121">
         <f>SUM(S21:T22)-U21</f>
         <v>1425.3699999999994</v>
       </c>
@@ -14757,11 +14757,11 @@
     </row>
     <row r="22" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A22" s="21"/>
-      <c r="B22" s="140" t="s">
+      <c r="B22" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="126"/>
-      <c r="D22" s="127" t="str">
+      <c r="C22" s="119"/>
+      <c r="D22" s="120" t="str">
         <f>D21</f>
         <v>Зырянов Д.Н.</v>
       </c>
@@ -14817,24 +14817,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S22" s="122"/>
-      <c r="T22" s="122"/>
-      <c r="U22" s="122"/>
-      <c r="V22" s="122"/>
+      <c r="S22" s="121"/>
+      <c r="T22" s="121"/>
+      <c r="U22" s="121"/>
+      <c r="V22" s="121"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
     </row>
     <row r="23" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A23" s="21"/>
-      <c r="B23" s="140">
+      <c r="B23" s="118">
         <f>Архив!A15</f>
         <v>8</v>
       </c>
-      <c r="C23" s="126">
+      <c r="C23" s="119">
         <f>Архив!G15</f>
         <v>44</v>
       </c>
-      <c r="D23" s="127" t="str">
+      <c r="D23" s="120" t="str">
         <f>Архив!B15</f>
         <v>Кавун А.И.</v>
       </c>
@@ -14890,19 +14890,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S23" s="122">
+      <c r="S23" s="121">
         <f>ROUND(SUM(P23:R24),2)</f>
         <v>1066.96</v>
       </c>
-      <c r="T23" s="122">
+      <c r="T23" s="121">
         <f>Архив!E15</f>
         <v>1643.1200000000008</v>
       </c>
-      <c r="U23" s="122">
+      <c r="U23" s="121">
         <f>Архив!F15</f>
         <v>6643</v>
       </c>
-      <c r="V23" s="122">
+      <c r="V23" s="121">
         <f>SUM(S23:T24)-U23</f>
         <v>-3932.9199999999992</v>
       </c>
@@ -14911,11 +14911,11 @@
     </row>
     <row r="24" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A24" s="21"/>
-      <c r="B24" s="140" t="s">
+      <c r="B24" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="126"/>
-      <c r="D24" s="127" t="str">
+      <c r="C24" s="119"/>
+      <c r="D24" s="120" t="str">
         <f>D23</f>
         <v>Кавун А.И.</v>
       </c>
@@ -14971,24 +14971,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S24" s="122"/>
-      <c r="T24" s="122"/>
-      <c r="U24" s="122"/>
-      <c r="V24" s="122"/>
+      <c r="S24" s="121"/>
+      <c r="T24" s="121"/>
+      <c r="U24" s="121"/>
+      <c r="V24" s="121"/>
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
     </row>
     <row r="25" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A25" s="21"/>
-      <c r="B25" s="140">
+      <c r="B25" s="118">
         <f>Архив!A17</f>
         <v>9</v>
       </c>
-      <c r="C25" s="126">
+      <c r="C25" s="119">
         <f>Архив!G17</f>
         <v>22</v>
       </c>
-      <c r="D25" s="127" t="str">
+      <c r="D25" s="120" t="str">
         <f>Архив!B17</f>
         <v>Калашников В.В.</v>
       </c>
@@ -15044,19 +15044,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S25" s="122">
+      <c r="S25" s="121">
         <f>ROUND(SUM(P25:R26),2)</f>
         <v>157.13</v>
       </c>
-      <c r="T25" s="122">
+      <c r="T25" s="121">
         <f>Архив!E17</f>
         <v>529.91000000000042</v>
       </c>
-      <c r="U25" s="122">
+      <c r="U25" s="121">
         <f>Архив!F17</f>
         <v>0</v>
       </c>
-      <c r="V25" s="122">
+      <c r="V25" s="121">
         <f>SUM(S25:T26)-U25</f>
         <v>687.04000000000042</v>
       </c>
@@ -15065,11 +15065,11 @@
     </row>
     <row r="26" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A26" s="21"/>
-      <c r="B26" s="140" t="s">
+      <c r="B26" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="126"/>
-      <c r="D26" s="127" t="str">
+      <c r="C26" s="119"/>
+      <c r="D26" s="120" t="str">
         <f>D25</f>
         <v>Калашников В.В.</v>
       </c>
@@ -15125,24 +15125,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S26" s="122"/>
-      <c r="T26" s="122"/>
-      <c r="U26" s="122"/>
-      <c r="V26" s="122"/>
+      <c r="S26" s="121"/>
+      <c r="T26" s="121"/>
+      <c r="U26" s="121"/>
+      <c r="V26" s="121"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
     </row>
     <row r="27" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A27" s="21"/>
-      <c r="B27" s="140">
+      <c r="B27" s="118">
         <f>Архив!A19</f>
         <v>10</v>
       </c>
-      <c r="C27" s="126">
+      <c r="C27" s="119">
         <f>Архив!G19</f>
         <v>8</v>
       </c>
-      <c r="D27" s="127" t="str">
+      <c r="D27" s="120" t="str">
         <f>Архив!B19</f>
         <v>Картира Я.А.</v>
       </c>
@@ -15198,19 +15198,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S27" s="122">
+      <c r="S27" s="121">
         <f>ROUND(SUM(P27:R28),2)</f>
         <v>920.28</v>
       </c>
-      <c r="T27" s="122">
+      <c r="T27" s="121">
         <f>Архив!E19</f>
         <v>1205.5</v>
       </c>
-      <c r="U27" s="122">
+      <c r="U27" s="121">
         <f>Архив!F19</f>
         <v>0</v>
       </c>
-      <c r="V27" s="122">
+      <c r="V27" s="121">
         <f>SUM(S27:T28)-U27</f>
         <v>2125.7799999999997</v>
       </c>
@@ -15219,11 +15219,11 @@
     </row>
     <row r="28" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="140" t="s">
+      <c r="B28" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="126"/>
-      <c r="D28" s="127" t="str">
+      <c r="C28" s="119"/>
+      <c r="D28" s="120" t="str">
         <f>D27</f>
         <v>Картира Я.А.</v>
       </c>
@@ -15279,24 +15279,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S28" s="122"/>
-      <c r="T28" s="122"/>
-      <c r="U28" s="122"/>
-      <c r="V28" s="122"/>
+      <c r="S28" s="121"/>
+      <c r="T28" s="121"/>
+      <c r="U28" s="121"/>
+      <c r="V28" s="121"/>
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
     </row>
     <row r="29" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A29" s="21"/>
-      <c r="B29" s="140">
+      <c r="B29" s="118">
         <f>Архив!A21</f>
         <v>11</v>
       </c>
-      <c r="C29" s="126">
+      <c r="C29" s="119">
         <f>Архив!G21</f>
         <v>36</v>
       </c>
-      <c r="D29" s="127" t="str">
+      <c r="D29" s="120" t="str">
         <f>Архив!B21</f>
         <v>Касьяненко А.А.</v>
       </c>
@@ -15352,19 +15352,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S29" s="122">
+      <c r="S29" s="121">
         <f>ROUND(SUM(P29:R30),2)</f>
         <v>1300.26</v>
       </c>
-      <c r="T29" s="122">
+      <c r="T29" s="121">
         <f>Архив!E21</f>
         <v>-53.740000000000009</v>
       </c>
-      <c r="U29" s="122">
+      <c r="U29" s="121">
         <f>Архив!F21</f>
         <v>1310</v>
       </c>
-      <c r="V29" s="122">
+      <c r="V29" s="121">
         <f>SUM(S29:T30)-U29</f>
         <v>-63.480000000000018</v>
       </c>
@@ -15373,11 +15373,11 @@
     </row>
     <row r="30" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A30" s="21"/>
-      <c r="B30" s="140" t="s">
+      <c r="B30" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="126"/>
-      <c r="D30" s="127" t="str">
+      <c r="C30" s="119"/>
+      <c r="D30" s="120" t="str">
         <f>D29</f>
         <v>Касьяненко А.А.</v>
       </c>
@@ -15433,24 +15433,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S30" s="122"/>
-      <c r="T30" s="122"/>
-      <c r="U30" s="122"/>
-      <c r="V30" s="122"/>
+      <c r="S30" s="121"/>
+      <c r="T30" s="121"/>
+      <c r="U30" s="121"/>
+      <c r="V30" s="121"/>
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
     </row>
     <row r="31" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="140">
+      <c r="B31" s="118">
         <f>Архив!A23</f>
         <v>12</v>
       </c>
-      <c r="C31" s="126">
+      <c r="C31" s="119">
         <f>Архив!G23</f>
         <v>18</v>
       </c>
-      <c r="D31" s="134" t="str">
+      <c r="D31" s="122" t="str">
         <f>Архив!B23</f>
         <v>Ким Т.В.</v>
       </c>
@@ -15506,15 +15506,15 @@
         <f t="shared" si="3"/>
         <v>3187.998660842346</v>
       </c>
-      <c r="S31" s="122">
+      <c r="S31" s="121">
         <f>ROUND(SUM(P31:R32),2)</f>
         <v>6900.05</v>
       </c>
-      <c r="T31" s="122">
+      <c r="T31" s="121">
         <f>Архив!E23</f>
         <v>0</v>
       </c>
-      <c r="U31" s="122">
+      <c r="U31" s="121">
         <f>Архив!F23</f>
         <v>0</v>
       </c>
@@ -15527,11 +15527,11 @@
     </row>
     <row r="32" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A32" s="21"/>
-      <c r="B32" s="140" t="s">
+      <c r="B32" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="126"/>
-      <c r="D32" s="134" t="str">
+      <c r="C32" s="119"/>
+      <c r="D32" s="122" t="str">
         <f>D31</f>
         <v>Ким Т.В.</v>
       </c>
@@ -15587,24 +15587,24 @@
         <f t="shared" si="3"/>
         <v>668.18253199064418</v>
       </c>
-      <c r="S32" s="122"/>
-      <c r="T32" s="122"/>
-      <c r="U32" s="122"/>
+      <c r="S32" s="121"/>
+      <c r="T32" s="121"/>
+      <c r="U32" s="121"/>
       <c r="V32" s="125"/>
       <c r="W32" s="6"/>
       <c r="X32" s="6"/>
     </row>
     <row r="33" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="140">
+      <c r="B33" s="118">
         <f>Архив!A25</f>
         <v>13</v>
       </c>
-      <c r="C33" s="126">
+      <c r="C33" s="119">
         <f>Архив!G25</f>
         <v>2</v>
       </c>
-      <c r="D33" s="127" t="str">
+      <c r="D33" s="120" t="str">
         <f>Архив!B25</f>
         <v>Клокова Е.В.</v>
       </c>
@@ -15660,19 +15660,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S33" s="122">
+      <c r="S33" s="121">
         <f>ROUND(SUM(P33:R34),2)</f>
         <v>1814.93</v>
       </c>
-      <c r="T33" s="122">
+      <c r="T33" s="121">
         <f>Архив!E25</f>
         <v>2920.6900000000005</v>
       </c>
-      <c r="U33" s="122">
+      <c r="U33" s="121">
         <f>Архив!F25</f>
         <v>3000</v>
       </c>
-      <c r="V33" s="122">
+      <c r="V33" s="121">
         <f>SUM(S33:T34)-U33</f>
         <v>1735.6200000000008</v>
       </c>
@@ -15681,11 +15681,11 @@
     </row>
     <row r="34" spans="1:24" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="140" t="s">
+      <c r="B34" s="118" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="126"/>
-      <c r="D34" s="127" t="str">
+      <c r="C34" s="119"/>
+      <c r="D34" s="120" t="str">
         <f>D33</f>
         <v>Клокова Е.В.</v>
       </c>
@@ -15741,24 +15741,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S34" s="122"/>
-      <c r="T34" s="122"/>
-      <c r="U34" s="122"/>
-      <c r="V34" s="122"/>
+      <c r="S34" s="121"/>
+      <c r="T34" s="121"/>
+      <c r="U34" s="121"/>
+      <c r="V34" s="121"/>
       <c r="W34" s="6"/>
       <c r="X34" s="6"/>
     </row>
     <row r="35" spans="1:24" ht="9.75" customHeight="1">
       <c r="A35" s="7"/>
-      <c r="B35" s="140">
+      <c r="B35" s="118">
         <f>Архив!A27</f>
         <v>14</v>
       </c>
-      <c r="C35" s="126">
+      <c r="C35" s="119">
         <f>Архив!G27</f>
         <v>9</v>
       </c>
-      <c r="D35" s="127" t="str">
+      <c r="D35" s="120" t="str">
         <f>Архив!B27</f>
         <v>Коваленко Р.Т.</v>
       </c>
@@ -15814,19 +15814,19 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S35" s="122">
+      <c r="S35" s="121">
         <f>ROUND(SUM(P35:R36),2)</f>
         <v>9.9</v>
       </c>
-      <c r="T35" s="122">
+      <c r="T35" s="121">
         <f>Архив!E27</f>
         <v>-63.18</v>
       </c>
-      <c r="U35" s="122">
+      <c r="U35" s="121">
         <f>Архив!F27</f>
         <v>100</v>
       </c>
-      <c r="V35" s="122">
+      <c r="V35" s="121">
         <f>SUM(S35:T36)-U35</f>
         <v>-153.28</v>
       </c>
@@ -15835,11 +15835,11 @@
     </row>
     <row r="36" spans="1:24" ht="9.75" customHeight="1">
       <c r="A36" s="7"/>
-      <c r="B36" s="140" t="s">
+      <c r="B36" s="118" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="126"/>
-      <c r="D36" s="127" t="str">
+      <c r="C36" s="119"/>
+      <c r="D36" s="120" t="str">
         <f>D35</f>
         <v>Коваленко Р.Т.</v>
       </c>
@@ -15895,24 +15895,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S36" s="122"/>
-      <c r="T36" s="122"/>
-      <c r="U36" s="122"/>
-      <c r="V36" s="122"/>
+      <c r="S36" s="121"/>
+      <c r="T36" s="121"/>
+      <c r="U36" s="121"/>
+      <c r="V36" s="121"/>
       <c r="W36" s="6"/>
       <c r="X36" s="6"/>
     </row>
     <row r="37" spans="1:24" ht="9.75" customHeight="1">
       <c r="A37" s="2"/>
-      <c r="B37" s="140">
+      <c r="B37" s="118">
         <f>Архив!A29</f>
         <v>15</v>
       </c>
-      <c r="C37" s="126">
+      <c r="C37" s="119">
         <f>Архив!G29</f>
         <v>15</v>
       </c>
-      <c r="D37" s="127" t="str">
+      <c r="D37" s="120" t="str">
         <f>Архив!B29</f>
         <v>Кралькина И.А.</v>
       </c>
@@ -15968,19 +15968,19 @@
         <f t="shared" si="3"/>
         <v>9640.2802568611278</v>
       </c>
-      <c r="S37" s="122">
+      <c r="S37" s="121">
         <f>ROUND(SUM(P37:R38),2)</f>
         <v>15498.81</v>
       </c>
-      <c r="T37" s="122">
+      <c r="T37" s="121">
         <f>Архив!E29</f>
         <v>16847.629999999997</v>
       </c>
-      <c r="U37" s="122">
+      <c r="U37" s="121">
         <f>Архив!F29</f>
         <v>16850</v>
       </c>
-      <c r="V37" s="122">
+      <c r="V37" s="121">
         <f>SUM(S37:T38)-U37</f>
         <v>15496.439999999995</v>
       </c>
@@ -15989,11 +15989,11 @@
     </row>
     <row r="38" spans="1:24" ht="9.75" customHeight="1">
       <c r="A38" s="2"/>
-      <c r="B38" s="140" t="s">
+      <c r="B38" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="126"/>
-      <c r="D38" s="127" t="str">
+      <c r="C38" s="119"/>
+      <c r="D38" s="120" t="str">
         <f>D37</f>
         <v>Кралькина И.А.</v>
       </c>
@@ -16049,24 +16049,24 @@
         <f t="shared" si="3"/>
         <v>2867.0762111213239</v>
       </c>
-      <c r="S38" s="122"/>
-      <c r="T38" s="122"/>
-      <c r="U38" s="122"/>
-      <c r="V38" s="122"/>
+      <c r="S38" s="121"/>
+      <c r="T38" s="121"/>
+      <c r="U38" s="121"/>
+      <c r="V38" s="121"/>
       <c r="W38" s="6"/>
       <c r="X38" s="6"/>
     </row>
     <row r="39" spans="1:24" ht="9.75" customHeight="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="140">
+      <c r="B39" s="118">
         <f>Архив!A31</f>
         <v>16</v>
       </c>
-      <c r="C39" s="126">
+      <c r="C39" s="119">
         <f>Архив!G31</f>
         <v>41</v>
       </c>
-      <c r="D39" s="134" t="str">
+      <c r="D39" s="122" t="str">
         <f>Архив!B31</f>
         <v>Кудряшов Ю.Ю.</v>
       </c>
@@ -16122,15 +16122,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S39" s="122">
+      <c r="S39" s="121">
         <f>ROUND(SUM(P39:R40),2)</f>
         <v>1581.33</v>
       </c>
-      <c r="T39" s="122">
+      <c r="T39" s="121">
         <f>Архив!E31</f>
         <v>4352.1000000000004</v>
       </c>
-      <c r="U39" s="122">
+      <c r="U39" s="121">
         <f>Архив!F31</f>
         <v>916.75</v>
       </c>
@@ -16143,11 +16143,11 @@
     </row>
     <row r="40" spans="1:24" ht="9.75" customHeight="1">
       <c r="A40" s="2"/>
-      <c r="B40" s="140" t="s">
+      <c r="B40" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="126"/>
-      <c r="D40" s="134" t="str">
+      <c r="C40" s="119"/>
+      <c r="D40" s="122" t="str">
         <f>D39</f>
         <v>Кудряшов Ю.Ю.</v>
       </c>
@@ -16203,9 +16203,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S40" s="122"/>
-      <c r="T40" s="122"/>
-      <c r="U40" s="122"/>
+      <c r="S40" s="121"/>
+      <c r="T40" s="121"/>
+      <c r="U40" s="121"/>
       <c r="V40" s="125"/>
       <c r="W40" s="6"/>
       <c r="X40" s="6"/>
@@ -16297,15 +16297,15 @@
     </row>
     <row r="42" spans="1:24" ht="9.75" customHeight="1">
       <c r="A42" s="2"/>
-      <c r="B42" s="140">
+      <c r="B42" s="118">
         <f>Архив!A34</f>
         <v>18</v>
       </c>
-      <c r="C42" s="126">
+      <c r="C42" s="119">
         <f>Архив!G34</f>
         <v>7</v>
       </c>
-      <c r="D42" s="127" t="str">
+      <c r="D42" s="120" t="str">
         <f>Архив!B34</f>
         <v>Лисина H.А.</v>
       </c>
@@ -16361,19 +16361,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S42" s="122">
+      <c r="S42" s="121">
         <f>ROUND(SUM(P42:R43),2)</f>
         <v>834.68</v>
       </c>
-      <c r="T42" s="122">
+      <c r="T42" s="121">
         <f>Архив!E34</f>
         <v>2158.2399999999998</v>
       </c>
-      <c r="U42" s="122">
+      <c r="U42" s="121">
         <f>Архив!F34</f>
         <v>2158.2399999999998</v>
       </c>
-      <c r="V42" s="122">
+      <c r="V42" s="121">
         <f>SUM(S42:T43)-U42</f>
         <v>834.67999999999984</v>
       </c>
@@ -16382,11 +16382,11 @@
     </row>
     <row r="43" spans="1:24" ht="9.75" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="140">
+      <c r="B43" s="118">
         <v>19</v>
       </c>
-      <c r="C43" s="126"/>
-      <c r="D43" s="127" t="str">
+      <c r="C43" s="119"/>
+      <c r="D43" s="120" t="str">
         <f>D42</f>
         <v>Лисина H.А.</v>
       </c>
@@ -16442,24 +16442,24 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S43" s="122"/>
-      <c r="T43" s="122"/>
-      <c r="U43" s="122"/>
-      <c r="V43" s="122"/>
+      <c r="S43" s="121"/>
+      <c r="T43" s="121"/>
+      <c r="U43" s="121"/>
+      <c r="V43" s="121"/>
       <c r="W43" s="6"/>
       <c r="X43" s="6"/>
     </row>
     <row r="44" spans="1:24" ht="9.75" customHeight="1">
       <c r="A44" s="2"/>
-      <c r="B44" s="140">
+      <c r="B44" s="118">
         <f>Архив!A36</f>
         <v>19</v>
       </c>
-      <c r="C44" s="126">
+      <c r="C44" s="119">
         <f>Архив!G36</f>
         <v>38</v>
       </c>
-      <c r="D44" s="127" t="str">
+      <c r="D44" s="120" t="str">
         <f>Архив!B36</f>
         <v>Лисина Н.А.</v>
       </c>
@@ -16515,19 +16515,19 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S44" s="122">
+      <c r="S44" s="121">
         <f>ROUND(SUM(P44:R45),2)</f>
         <v>115.74</v>
       </c>
-      <c r="T44" s="122">
+      <c r="T44" s="121">
         <f>Архив!E36</f>
         <v>415.72</v>
       </c>
-      <c r="U44" s="122">
+      <c r="U44" s="121">
         <f>Архив!F36</f>
         <v>415.72</v>
       </c>
-      <c r="V44" s="122">
+      <c r="V44" s="121">
         <f>SUM(S44:T44)-U44</f>
         <v>115.74000000000001</v>
       </c>
@@ -16536,11 +16536,11 @@
     </row>
     <row r="45" spans="1:24" ht="9.75" customHeight="1">
       <c r="A45" s="2"/>
-      <c r="B45" s="140">
+      <c r="B45" s="118">
         <v>20</v>
       </c>
-      <c r="C45" s="126"/>
-      <c r="D45" s="127" t="str">
+      <c r="C45" s="119"/>
+      <c r="D45" s="120" t="str">
         <f>D44</f>
         <v>Лисина Н.А.</v>
       </c>
@@ -16596,10 +16596,10 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S45" s="122"/>
-      <c r="T45" s="122"/>
-      <c r="U45" s="122"/>
-      <c r="V45" s="122"/>
+      <c r="S45" s="121"/>
+      <c r="T45" s="121"/>
+      <c r="U45" s="121"/>
+      <c r="V45" s="121"/>
       <c r="W45" s="6"/>
       <c r="X45" s="6"/>
     </row>
@@ -16690,15 +16690,15 @@
     </row>
     <row r="47" spans="1:24" ht="9.75" customHeight="1">
       <c r="A47" s="2"/>
-      <c r="B47" s="140">
+      <c r="B47" s="118">
         <f>Архив!A39</f>
         <v>21</v>
       </c>
-      <c r="C47" s="126">
+      <c r="C47" s="119">
         <f>Архив!G39</f>
         <v>31</v>
       </c>
-      <c r="D47" s="127" t="str">
+      <c r="D47" s="120" t="str">
         <f>Архив!B39</f>
         <v>Милакина М.В.</v>
       </c>
@@ -16754,19 +16754,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S47" s="122">
+      <c r="S47" s="121">
         <f>ROUND(SUM(P47:R48),2)</f>
         <v>2438.92</v>
       </c>
-      <c r="T47" s="122">
+      <c r="T47" s="121">
         <f>Архив!E39</f>
         <v>2064.5499999999993</v>
       </c>
-      <c r="U47" s="122">
+      <c r="U47" s="121">
         <f>Архив!F39</f>
         <v>4600</v>
       </c>
-      <c r="V47" s="122">
+      <c r="V47" s="121">
         <f>SUM(S47:T48)-U47</f>
         <v>-96.530000000000655</v>
       </c>
@@ -16775,11 +16775,11 @@
     </row>
     <row r="48" spans="1:24" ht="9.75" customHeight="1">
       <c r="A48" s="2"/>
-      <c r="B48" s="140">
+      <c r="B48" s="118">
         <v>22</v>
       </c>
-      <c r="C48" s="126"/>
-      <c r="D48" s="127" t="str">
+      <c r="C48" s="119"/>
+      <c r="D48" s="120" t="str">
         <f>D47</f>
         <v>Милакина М.В.</v>
       </c>
@@ -16835,24 +16835,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S48" s="122"/>
-      <c r="T48" s="122"/>
-      <c r="U48" s="122"/>
-      <c r="V48" s="122"/>
+      <c r="S48" s="121"/>
+      <c r="T48" s="121"/>
+      <c r="U48" s="121"/>
+      <c r="V48" s="121"/>
       <c r="W48" s="6"/>
       <c r="X48" s="6"/>
     </row>
     <row r="49" spans="1:24" ht="9.75" customHeight="1">
       <c r="A49" s="2"/>
-      <c r="B49" s="140">
+      <c r="B49" s="118">
         <f>Архив!A41</f>
         <v>22</v>
       </c>
-      <c r="C49" s="126">
+      <c r="C49" s="119">
         <f>Архив!G41</f>
         <v>11</v>
       </c>
-      <c r="D49" s="127" t="str">
+      <c r="D49" s="120" t="str">
         <f>Архив!B41</f>
         <v>Мирошниченко Л.В.</v>
       </c>
@@ -16908,19 +16908,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S49" s="122">
+      <c r="S49" s="121">
         <f>ROUND(SUM(P49:R50),2)</f>
         <v>793.98</v>
       </c>
-      <c r="T49" s="122">
+      <c r="T49" s="121">
         <f>Архив!E41</f>
         <v>1236.4899999999993</v>
       </c>
-      <c r="U49" s="122">
+      <c r="U49" s="121">
         <f>Архив!F41</f>
         <v>1236.49</v>
       </c>
-      <c r="V49" s="139">
+      <c r="V49" s="126">
         <f>SUM(S49:T50)-U49</f>
         <v>793.97999999999934</v>
       </c>
@@ -16929,11 +16929,11 @@
     </row>
     <row r="50" spans="1:24" ht="9.75" customHeight="1">
       <c r="A50" s="2"/>
-      <c r="B50" s="140">
+      <c r="B50" s="118">
         <v>23</v>
       </c>
-      <c r="C50" s="126"/>
-      <c r="D50" s="127" t="str">
+      <c r="C50" s="119"/>
+      <c r="D50" s="120" t="str">
         <f>D49</f>
         <v>Мирошниченко Л.В.</v>
       </c>
@@ -16989,24 +16989,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S50" s="122"/>
-      <c r="T50" s="122"/>
-      <c r="U50" s="122"/>
-      <c r="V50" s="139"/>
+      <c r="S50" s="121"/>
+      <c r="T50" s="121"/>
+      <c r="U50" s="121"/>
+      <c r="V50" s="126"/>
       <c r="W50" s="6"/>
       <c r="X50" s="6"/>
     </row>
     <row r="51" spans="1:24" ht="9.75" customHeight="1">
       <c r="A51" s="2"/>
-      <c r="B51" s="140">
+      <c r="B51" s="118">
         <f>Архив!A43</f>
         <v>23</v>
       </c>
-      <c r="C51" s="126">
+      <c r="C51" s="119">
         <f>Архив!G43</f>
         <v>58</v>
       </c>
-      <c r="D51" s="127" t="str">
+      <c r="D51" s="120" t="str">
         <f>Архив!B43</f>
         <v xml:space="preserve">Митрофанова И.В. </v>
       </c>
@@ -17062,19 +17062,19 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S51" s="122">
+      <c r="S51" s="121">
         <f>ROUND(SUM(P51:R52),2)</f>
         <v>0</v>
       </c>
-      <c r="T51" s="122">
+      <c r="T51" s="121">
         <f>Архив!E43</f>
         <v>0</v>
       </c>
-      <c r="U51" s="122">
+      <c r="U51" s="121">
         <f>Архив!F43</f>
         <v>0</v>
       </c>
-      <c r="V51" s="122">
+      <c r="V51" s="121">
         <f>SUM(S51:T52)-U51</f>
         <v>0</v>
       </c>
@@ -17083,11 +17083,11 @@
     </row>
     <row r="52" spans="1:24" ht="9.75" customHeight="1">
       <c r="A52" s="2"/>
-      <c r="B52" s="140">
+      <c r="B52" s="118">
         <v>24</v>
       </c>
-      <c r="C52" s="126"/>
-      <c r="D52" s="127" t="str">
+      <c r="C52" s="119"/>
+      <c r="D52" s="120" t="str">
         <f>D51</f>
         <v xml:space="preserve">Митрофанова И.В. </v>
       </c>
@@ -17143,10 +17143,10 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S52" s="122"/>
-      <c r="T52" s="122"/>
-      <c r="U52" s="122"/>
-      <c r="V52" s="122"/>
+      <c r="S52" s="121"/>
+      <c r="T52" s="121"/>
+      <c r="U52" s="121"/>
+      <c r="V52" s="121"/>
       <c r="W52" s="6"/>
       <c r="X52" s="6"/>
     </row>
@@ -17322,15 +17322,15 @@
     </row>
     <row r="55" spans="1:24" ht="9.75" customHeight="1">
       <c r="A55" s="2"/>
-      <c r="B55" s="140">
+      <c r="B55" s="118">
         <f>Архив!A47</f>
         <v>26</v>
       </c>
-      <c r="C55" s="126">
+      <c r="C55" s="119">
         <f>Архив!G47</f>
         <v>20</v>
       </c>
-      <c r="D55" s="127" t="str">
+      <c r="D55" s="120" t="str">
         <f>Архив!B47</f>
         <v>Ненахов С.А.</v>
       </c>
@@ -17386,19 +17386,19 @@
         <f t="shared" si="8"/>
         <v>2433.4217222896787</v>
       </c>
-      <c r="S55" s="122">
+      <c r="S55" s="121">
         <f>ROUND(SUM(P55:R56),2)</f>
         <v>6432.92</v>
       </c>
-      <c r="T55" s="122">
+      <c r="T55" s="121">
         <f>Архив!E47</f>
         <v>19047.41</v>
       </c>
-      <c r="U55" s="122">
+      <c r="U55" s="121">
         <f>Архив!F47</f>
         <v>19047.41</v>
       </c>
-      <c r="V55" s="139">
+      <c r="V55" s="126">
         <f>SUM(S55:T56)-U55</f>
         <v>6432.9200000000019</v>
       </c>
@@ -17407,11 +17407,11 @@
     </row>
     <row r="56" spans="1:24" ht="9.75" customHeight="1">
       <c r="A56" s="2"/>
-      <c r="B56" s="140">
+      <c r="B56" s="118">
         <v>27</v>
       </c>
-      <c r="C56" s="126"/>
-      <c r="D56" s="127" t="str">
+      <c r="C56" s="119"/>
+      <c r="D56" s="120" t="str">
         <f>D55</f>
         <v>Ненахов С.А.</v>
       </c>
@@ -17467,24 +17467,24 @@
         <f t="shared" si="8"/>
         <v>1077.8254873611838</v>
       </c>
-      <c r="S56" s="122"/>
-      <c r="T56" s="122"/>
-      <c r="U56" s="122"/>
-      <c r="V56" s="139"/>
+      <c r="S56" s="121"/>
+      <c r="T56" s="121"/>
+      <c r="U56" s="121"/>
+      <c r="V56" s="126"/>
       <c r="W56" s="6"/>
       <c r="X56" s="6"/>
     </row>
     <row r="57" spans="1:24" ht="9.75" customHeight="1">
       <c r="A57" s="2"/>
-      <c r="B57" s="140">
+      <c r="B57" s="118">
         <f>Архив!A49</f>
         <v>27</v>
       </c>
-      <c r="C57" s="126">
+      <c r="C57" s="119">
         <f>Архив!G49</f>
         <v>50</v>
       </c>
-      <c r="D57" s="127" t="str">
+      <c r="D57" s="120" t="str">
         <f>Архив!B49</f>
         <v>Новацкий О.В.</v>
       </c>
@@ -17540,19 +17540,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S57" s="122">
+      <c r="S57" s="121">
         <f>ROUND(SUM(P57:R58),2)</f>
         <v>1396.99</v>
       </c>
-      <c r="T57" s="122">
+      <c r="T57" s="121">
         <f>Архив!E49</f>
         <v>-47.769999999999527</v>
       </c>
-      <c r="U57" s="122">
+      <c r="U57" s="121">
         <f>Архив!F49</f>
         <v>1500</v>
       </c>
-      <c r="V57" s="122">
+      <c r="V57" s="121">
         <f>SUM(S57:T58)-U57</f>
         <v>-150.77999999999952</v>
       </c>
@@ -17561,11 +17561,11 @@
     </row>
     <row r="58" spans="1:24" ht="9.75" customHeight="1">
       <c r="A58" s="2"/>
-      <c r="B58" s="140">
+      <c r="B58" s="118">
         <v>28</v>
       </c>
-      <c r="C58" s="126"/>
-      <c r="D58" s="127" t="str">
+      <c r="C58" s="119"/>
+      <c r="D58" s="120" t="str">
         <f>D57</f>
         <v>Новацкий О.В.</v>
       </c>
@@ -17621,24 +17621,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S58" s="122"/>
-      <c r="T58" s="122"/>
-      <c r="U58" s="122"/>
-      <c r="V58" s="122"/>
+      <c r="S58" s="121"/>
+      <c r="T58" s="121"/>
+      <c r="U58" s="121"/>
+      <c r="V58" s="121"/>
       <c r="W58" s="6"/>
       <c r="X58" s="6"/>
     </row>
     <row r="59" spans="1:24" ht="9.75" customHeight="1">
       <c r="A59" s="2"/>
-      <c r="B59" s="140">
+      <c r="B59" s="118">
         <f>Архив!A51</f>
         <v>28</v>
       </c>
-      <c r="C59" s="126">
+      <c r="C59" s="119">
         <f>Архив!G51</f>
         <v>4</v>
       </c>
-      <c r="D59" s="127" t="str">
+      <c r="D59" s="120" t="str">
         <f>Архив!B51</f>
         <v>Носовский В.А.</v>
       </c>
@@ -17694,19 +17694,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S59" s="122">
+      <c r="S59" s="121">
         <f>ROUND(SUM(P59:R60),2)</f>
         <v>0.43</v>
       </c>
-      <c r="T59" s="122">
+      <c r="T59" s="121">
         <f>Архив!E51</f>
         <v>-302.7</v>
       </c>
-      <c r="U59" s="122">
+      <c r="U59" s="121">
         <f>Архив!F51</f>
         <v>0</v>
       </c>
-      <c r="V59" s="122">
+      <c r="V59" s="121">
         <f>SUM(S59:T60)-U59</f>
         <v>-302.27</v>
       </c>
@@ -17715,11 +17715,11 @@
     </row>
     <row r="60" spans="1:24" ht="9.75" customHeight="1">
       <c r="A60" s="2"/>
-      <c r="B60" s="140">
+      <c r="B60" s="118">
         <v>29</v>
       </c>
-      <c r="C60" s="126"/>
-      <c r="D60" s="127" t="str">
+      <c r="C60" s="119"/>
+      <c r="D60" s="120" t="str">
         <f>D59</f>
         <v>Носовский В.А.</v>
       </c>
@@ -17775,24 +17775,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S60" s="122"/>
-      <c r="T60" s="122"/>
-      <c r="U60" s="122"/>
-      <c r="V60" s="122"/>
+      <c r="S60" s="121"/>
+      <c r="T60" s="121"/>
+      <c r="U60" s="121"/>
+      <c r="V60" s="121"/>
       <c r="W60" s="6"/>
       <c r="X60" s="6"/>
     </row>
     <row r="61" spans="1:24" ht="9.75" customHeight="1">
       <c r="A61" s="2"/>
-      <c r="B61" s="140">
+      <c r="B61" s="118">
         <f>Архив!A53</f>
         <v>29</v>
       </c>
-      <c r="C61" s="126">
+      <c r="C61" s="119">
         <f>Архив!G53</f>
         <v>32</v>
       </c>
-      <c r="D61" s="127" t="str">
+      <c r="D61" s="120" t="str">
         <f>Архив!B53</f>
         <v>Ольшинецкий В.В.</v>
       </c>
@@ -17848,19 +17848,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S61" s="122">
+      <c r="S61" s="121">
         <f>ROUND(SUM(P61:R62),2)</f>
         <v>678.31</v>
       </c>
-      <c r="T61" s="122">
+      <c r="T61" s="121">
         <f>Архив!E53</f>
         <v>-49.889999999999816</v>
       </c>
-      <c r="U61" s="122">
+      <c r="U61" s="121">
         <f>Архив!F53</f>
         <v>1350</v>
       </c>
-      <c r="V61" s="122">
+      <c r="V61" s="121">
         <f>SUM(S61:T62)-U61</f>
         <v>-721.57999999999993</v>
       </c>
@@ -17869,11 +17869,11 @@
     </row>
     <row r="62" spans="1:24" ht="9.75" customHeight="1">
       <c r="A62" s="2"/>
-      <c r="B62" s="140">
+      <c r="B62" s="118">
         <v>30</v>
       </c>
-      <c r="C62" s="126"/>
-      <c r="D62" s="127" t="str">
+      <c r="C62" s="119"/>
+      <c r="D62" s="120" t="str">
         <f>D61</f>
         <v>Ольшинецкий В.В.</v>
       </c>
@@ -17929,10 +17929,10 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S62" s="122"/>
-      <c r="T62" s="122"/>
-      <c r="U62" s="122"/>
-      <c r="V62" s="122"/>
+      <c r="S62" s="121"/>
+      <c r="T62" s="121"/>
+      <c r="U62" s="121"/>
+      <c r="V62" s="121"/>
       <c r="W62" s="6"/>
       <c r="X62" s="6"/>
     </row>
@@ -18023,15 +18023,15 @@
     </row>
     <row r="64" spans="1:24" ht="9.75" customHeight="1">
       <c r="A64" s="2"/>
-      <c r="B64" s="140">
+      <c r="B64" s="118">
         <f>Архив!A56</f>
         <v>31</v>
       </c>
-      <c r="C64" s="126">
+      <c r="C64" s="119">
         <f>Архив!G56</f>
         <v>33</v>
       </c>
-      <c r="D64" s="127" t="str">
+      <c r="D64" s="120" t="str">
         <f>Архив!B56</f>
         <v>Пильник А.Я.</v>
       </c>
@@ -18087,19 +18087,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S64" s="122">
+      <c r="S64" s="121">
         <f>ROUND(SUM(P64:R65),2)</f>
         <v>1974.04</v>
       </c>
-      <c r="T64" s="122">
+      <c r="T64" s="121">
         <f>Архив!E56</f>
         <v>2665.42</v>
       </c>
-      <c r="U64" s="122">
+      <c r="U64" s="121">
         <f>Архив!F56</f>
         <v>2665.42</v>
       </c>
-      <c r="V64" s="122">
+      <c r="V64" s="121">
         <f>SUM(S64:T65)-U64</f>
         <v>1974.04</v>
       </c>
@@ -18108,11 +18108,11 @@
     </row>
     <row r="65" spans="1:24" ht="9.75" customHeight="1">
       <c r="A65" s="2"/>
-      <c r="B65" s="140">
+      <c r="B65" s="118">
         <v>32</v>
       </c>
-      <c r="C65" s="126"/>
-      <c r="D65" s="127" t="str">
+      <c r="C65" s="119"/>
+      <c r="D65" s="120" t="str">
         <f>D64</f>
         <v>Пильник А.Я.</v>
       </c>
@@ -18168,24 +18168,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S65" s="122"/>
-      <c r="T65" s="122"/>
-      <c r="U65" s="122"/>
-      <c r="V65" s="122"/>
+      <c r="S65" s="121"/>
+      <c r="T65" s="121"/>
+      <c r="U65" s="121"/>
+      <c r="V65" s="121"/>
       <c r="W65" s="6"/>
       <c r="X65" s="6"/>
     </row>
     <row r="66" spans="1:24" ht="9.75" customHeight="1">
       <c r="A66" s="2"/>
-      <c r="B66" s="140">
+      <c r="B66" s="118">
         <f>Архив!A58</f>
         <v>32</v>
       </c>
-      <c r="C66" s="126">
+      <c r="C66" s="119">
         <f>Архив!G58</f>
         <v>34</v>
       </c>
-      <c r="D66" s="127" t="str">
+      <c r="D66" s="120" t="str">
         <f>Архив!B58</f>
         <v>Рок М.В.</v>
       </c>
@@ -18241,19 +18241,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S66" s="122">
+      <c r="S66" s="121">
         <f>ROUND(SUM(P66:R67),2)</f>
         <v>204.31</v>
       </c>
-      <c r="T66" s="122">
+      <c r="T66" s="121">
         <f>Архив!E58</f>
         <v>-305.71999999999991</v>
       </c>
-      <c r="U66" s="122">
+      <c r="U66" s="121">
         <f>Архив!F58</f>
         <v>1000</v>
       </c>
-      <c r="V66" s="122">
+      <c r="V66" s="121">
         <f>SUM(S66:T67)-U66</f>
         <v>-1101.4099999999999</v>
       </c>
@@ -18262,11 +18262,11 @@
     </row>
     <row r="67" spans="1:24" ht="9.75" customHeight="1">
       <c r="A67" s="2"/>
-      <c r="B67" s="140">
+      <c r="B67" s="118">
         <v>33</v>
       </c>
-      <c r="C67" s="126"/>
-      <c r="D67" s="127" t="str">
+      <c r="C67" s="119"/>
+      <c r="D67" s="120" t="str">
         <f>D66</f>
         <v>Рок М.В.</v>
       </c>
@@ -18322,24 +18322,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S67" s="122"/>
-      <c r="T67" s="122"/>
-      <c r="U67" s="122"/>
-      <c r="V67" s="122"/>
+      <c r="S67" s="121"/>
+      <c r="T67" s="121"/>
+      <c r="U67" s="121"/>
+      <c r="V67" s="121"/>
       <c r="W67" s="6"/>
       <c r="X67" s="6"/>
     </row>
     <row r="68" spans="1:24" ht="9.75" customHeight="1">
       <c r="A68" s="2"/>
-      <c r="B68" s="140">
+      <c r="B68" s="118">
         <f>Архив!A60</f>
         <v>33</v>
       </c>
-      <c r="C68" s="126" t="str">
+      <c r="C68" s="119" t="str">
         <f>Архив!G60</f>
         <v>56-А</v>
       </c>
-      <c r="D68" s="127" t="str">
+      <c r="D68" s="120" t="str">
         <f>Архив!B60</f>
         <v>Рубцова Т.В.</v>
       </c>
@@ -18395,19 +18395,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S68" s="122">
+      <c r="S68" s="121">
         <f>ROUND(SUM(P68:R69),2)</f>
         <v>1922.64</v>
       </c>
-      <c r="T68" s="122">
+      <c r="T68" s="121">
         <f>Архив!E60</f>
         <v>2444.6499999999996</v>
       </c>
-      <c r="U68" s="122">
+      <c r="U68" s="121">
         <f>Архив!F60</f>
         <v>2000</v>
       </c>
-      <c r="V68" s="139">
+      <c r="V68" s="126">
         <f>SUM(S68:T69)-U68</f>
         <v>2367.29</v>
       </c>
@@ -18416,11 +18416,11 @@
     </row>
     <row r="69" spans="1:24" ht="9.75" customHeight="1">
       <c r="A69" s="2"/>
-      <c r="B69" s="140">
+      <c r="B69" s="118">
         <v>34</v>
       </c>
-      <c r="C69" s="126"/>
-      <c r="D69" s="127" t="str">
+      <c r="C69" s="119"/>
+      <c r="D69" s="120" t="str">
         <f>D68</f>
         <v>Рубцова Т.В.</v>
       </c>
@@ -18476,24 +18476,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S69" s="122"/>
-      <c r="T69" s="122"/>
-      <c r="U69" s="122"/>
-      <c r="V69" s="139"/>
+      <c r="S69" s="121"/>
+      <c r="T69" s="121"/>
+      <c r="U69" s="121"/>
+      <c r="V69" s="126"/>
       <c r="W69" s="6"/>
       <c r="X69" s="6"/>
     </row>
     <row r="70" spans="1:24" ht="9.75" customHeight="1">
       <c r="A70" s="2"/>
-      <c r="B70" s="140">
+      <c r="B70" s="118">
         <f>Архив!A62</f>
         <v>34</v>
       </c>
-      <c r="C70" s="126">
+      <c r="C70" s="119">
         <f>Архив!G62</f>
         <v>37</v>
       </c>
-      <c r="D70" s="127" t="str">
+      <c r="D70" s="120" t="str">
         <f>Архив!B62</f>
         <v>Самойленко С.Б.</v>
       </c>
@@ -18549,19 +18549,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S70" s="122">
+      <c r="S70" s="121">
         <f>ROUND(SUM(P70:R71),2)</f>
         <v>2020.37</v>
       </c>
-      <c r="T70" s="122">
+      <c r="T70" s="121">
         <f>Архив!E62</f>
         <v>2131.5500000000002</v>
       </c>
-      <c r="U70" s="122">
+      <c r="U70" s="121">
         <f>Архив!F62</f>
         <v>2200</v>
       </c>
-      <c r="V70" s="122">
+      <c r="V70" s="121">
         <f>SUM(S70:T71)-U70</f>
         <v>1951.92</v>
       </c>
@@ -18570,11 +18570,11 @@
     </row>
     <row r="71" spans="1:24" ht="9.75" customHeight="1">
       <c r="A71" s="2"/>
-      <c r="B71" s="140">
+      <c r="B71" s="118">
         <v>35</v>
       </c>
-      <c r="C71" s="126"/>
-      <c r="D71" s="127" t="str">
+      <c r="C71" s="119"/>
+      <c r="D71" s="120" t="str">
         <f>D70</f>
         <v>Самойленко С.Б.</v>
       </c>
@@ -18630,24 +18630,24 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S71" s="122"/>
-      <c r="T71" s="122"/>
-      <c r="U71" s="122"/>
-      <c r="V71" s="122"/>
+      <c r="S71" s="121"/>
+      <c r="T71" s="121"/>
+      <c r="U71" s="121"/>
+      <c r="V71" s="121"/>
       <c r="W71" s="6"/>
       <c r="X71" s="6"/>
     </row>
     <row r="72" spans="1:24" ht="9.75" customHeight="1">
       <c r="A72" s="2"/>
-      <c r="B72" s="140">
+      <c r="B72" s="118">
         <f>Архив!A64</f>
         <v>35</v>
       </c>
-      <c r="C72" s="126">
+      <c r="C72" s="119">
         <f>Архив!G64</f>
         <v>29</v>
       </c>
-      <c r="D72" s="127" t="str">
+      <c r="D72" s="120" t="str">
         <f>Архив!B64</f>
         <v>Сидорец А.С.</v>
       </c>
@@ -18703,19 +18703,19 @@
         <f t="shared" ref="R72:R89" si="13">IF(L72&lt;0,0,L72*O72)</f>
         <v>0</v>
       </c>
-      <c r="S72" s="122">
+      <c r="S72" s="121">
         <f>ROUND(SUM(P72:R73),2)</f>
         <v>1226.44</v>
       </c>
-      <c r="T72" s="122">
+      <c r="T72" s="121">
         <f>Архив!E64</f>
         <v>2110.4499999999998</v>
       </c>
-      <c r="U72" s="122">
+      <c r="U72" s="121">
         <f>Архив!F64</f>
         <v>2110.4499999999998</v>
       </c>
-      <c r="V72" s="122">
+      <c r="V72" s="121">
         <f>SUM(S72:T73)-U72</f>
         <v>1226.44</v>
       </c>
@@ -18724,11 +18724,11 @@
     </row>
     <row r="73" spans="1:24" ht="9.75" customHeight="1">
       <c r="A73" s="2"/>
-      <c r="B73" s="140">
+      <c r="B73" s="118">
         <v>36</v>
       </c>
-      <c r="C73" s="126"/>
-      <c r="D73" s="127" t="str">
+      <c r="C73" s="119"/>
+      <c r="D73" s="120" t="str">
         <f>D72</f>
         <v>Сидорец А.С.</v>
       </c>
@@ -18784,10 +18784,10 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S73" s="122"/>
-      <c r="T73" s="122"/>
-      <c r="U73" s="122"/>
-      <c r="V73" s="122"/>
+      <c r="S73" s="121"/>
+      <c r="T73" s="121"/>
+      <c r="U73" s="121"/>
+      <c r="V73" s="121"/>
       <c r="W73" s="6"/>
       <c r="X73" s="6"/>
     </row>
@@ -18878,15 +18878,15 @@
     </row>
     <row r="75" spans="1:24" ht="9.75" customHeight="1">
       <c r="A75" s="2"/>
-      <c r="B75" s="140">
+      <c r="B75" s="118">
         <f>Архив!A67</f>
         <v>37</v>
       </c>
-      <c r="C75" s="126">
+      <c r="C75" s="119">
         <f>Архив!G67</f>
         <v>30</v>
       </c>
-      <c r="D75" s="127" t="str">
+      <c r="D75" s="120" t="str">
         <f>Архив!B67</f>
         <v>Смирнов С.В.</v>
       </c>
@@ -18942,19 +18942,19 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S75" s="122">
+      <c r="S75" s="121">
         <f>ROUND(SUM(P75:R76),2)</f>
         <v>1168.83</v>
       </c>
-      <c r="T75" s="122">
+      <c r="T75" s="121">
         <f>Архив!E67</f>
         <v>3060.6</v>
       </c>
-      <c r="U75" s="122">
+      <c r="U75" s="121">
         <f>Архив!F67</f>
         <v>0</v>
       </c>
-      <c r="V75" s="122">
+      <c r="V75" s="121">
         <f>SUM(S75:T76)-U75</f>
         <v>4229.43</v>
       </c>
@@ -18963,11 +18963,11 @@
     </row>
     <row r="76" spans="1:24" ht="9.75" customHeight="1">
       <c r="A76" s="2"/>
-      <c r="B76" s="140">
+      <c r="B76" s="118">
         <v>38</v>
       </c>
-      <c r="C76" s="126"/>
-      <c r="D76" s="127" t="str">
+      <c r="C76" s="119"/>
+      <c r="D76" s="120" t="str">
         <f>D75</f>
         <v>Смирнов С.В.</v>
       </c>
@@ -19023,24 +19023,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S76" s="122"/>
-      <c r="T76" s="122"/>
-      <c r="U76" s="122"/>
-      <c r="V76" s="122"/>
+      <c r="S76" s="121"/>
+      <c r="T76" s="121"/>
+      <c r="U76" s="121"/>
+      <c r="V76" s="121"/>
       <c r="W76" s="6"/>
       <c r="X76" s="6"/>
     </row>
     <row r="77" spans="1:24" ht="9.75" customHeight="1">
       <c r="A77" s="2"/>
-      <c r="B77" s="140">
+      <c r="B77" s="118">
         <f>Архив!A69</f>
         <v>38</v>
       </c>
-      <c r="C77" s="126" t="str">
+      <c r="C77" s="119" t="str">
         <f>Архив!G69</f>
-        <v>53/а</v>
-      </c>
-      <c r="D77" s="127" t="str">
+        <v>53-а</v>
+      </c>
+      <c r="D77" s="120" t="str">
         <f>Архив!B69</f>
         <v>Трактин В.В.</v>
       </c>
@@ -19096,19 +19096,19 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S77" s="122">
+      <c r="S77" s="121">
         <f>ROUND(SUM(P77:R78),2)</f>
         <v>2094.59</v>
       </c>
-      <c r="T77" s="122">
+      <c r="T77" s="121">
         <f>Архив!E69</f>
         <v>15802.539999999994</v>
       </c>
-      <c r="U77" s="122">
+      <c r="U77" s="121">
         <f>Архив!F69</f>
         <v>15802.54</v>
       </c>
-      <c r="V77" s="122">
+      <c r="V77" s="121">
         <f>SUM(S77:T78)-U77</f>
         <v>2094.5899999999929</v>
       </c>
@@ -19117,11 +19117,11 @@
     </row>
     <row r="78" spans="1:24" ht="9.75" customHeight="1">
       <c r="A78" s="2"/>
-      <c r="B78" s="140">
+      <c r="B78" s="118">
         <v>39</v>
       </c>
-      <c r="C78" s="126"/>
-      <c r="D78" s="127" t="str">
+      <c r="C78" s="119"/>
+      <c r="D78" s="120" t="str">
         <f>D77</f>
         <v>Трактин В.В.</v>
       </c>
@@ -19177,24 +19177,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S78" s="122"/>
-      <c r="T78" s="122"/>
-      <c r="U78" s="122"/>
-      <c r="V78" s="122"/>
+      <c r="S78" s="121"/>
+      <c r="T78" s="121"/>
+      <c r="U78" s="121"/>
+      <c r="V78" s="121"/>
       <c r="W78" s="6"/>
       <c r="X78" s="6"/>
     </row>
     <row r="79" spans="1:24" ht="9.75" customHeight="1">
       <c r="A79" s="2"/>
-      <c r="B79" s="140">
+      <c r="B79" s="118">
         <f>Архив!A71</f>
         <v>39</v>
       </c>
-      <c r="C79" s="126" t="str">
+      <c r="C79" s="119" t="str">
         <f>Архив!G71</f>
-        <v>53/б</v>
-      </c>
-      <c r="D79" s="127" t="str">
+        <v>53-б</v>
+      </c>
+      <c r="D79" s="120" t="str">
         <f>Архив!B71</f>
         <v>Трактин Р.В.</v>
       </c>
@@ -19250,19 +19250,19 @@
         <f>IF(L79&lt;0,0,L79*O79)</f>
         <v>1019.0930277247502</v>
       </c>
-      <c r="S79" s="122">
+      <c r="S79" s="121">
         <f>ROUND(SUM(P79:R80),2)</f>
         <v>4470.93</v>
       </c>
-      <c r="T79" s="122">
+      <c r="T79" s="121">
         <f>Архив!E71</f>
         <v>3236.9100000000008</v>
       </c>
-      <c r="U79" s="122">
+      <c r="U79" s="121">
         <f>Архив!F71</f>
         <v>3236.91</v>
       </c>
-      <c r="V79" s="122">
+      <c r="V79" s="121">
         <f>SUM(S79:T80)-U79</f>
         <v>4470.9300000000012</v>
       </c>
@@ -19271,11 +19271,11 @@
     </row>
     <row r="80" spans="1:24" ht="9.75" customHeight="1">
       <c r="A80" s="2"/>
-      <c r="B80" s="140">
+      <c r="B80" s="118">
         <v>40</v>
       </c>
-      <c r="C80" s="126"/>
-      <c r="D80" s="127" t="str">
+      <c r="C80" s="119"/>
+      <c r="D80" s="120" t="str">
         <f>D79</f>
         <v>Трактин Р.В.</v>
       </c>
@@ -19331,10 +19331,10 @@
         <f>IF(L80&lt;0,0,L80*O80)</f>
         <v>577.20517831957432</v>
       </c>
-      <c r="S80" s="122"/>
-      <c r="T80" s="122"/>
-      <c r="U80" s="122"/>
-      <c r="V80" s="122"/>
+      <c r="S80" s="121"/>
+      <c r="T80" s="121"/>
+      <c r="U80" s="121"/>
+      <c r="V80" s="121"/>
       <c r="W80" s="6"/>
       <c r="X80" s="6"/>
     </row>
@@ -19425,15 +19425,15 @@
     </row>
     <row r="82" spans="1:24" ht="9.75" customHeight="1">
       <c r="A82" s="2"/>
-      <c r="B82" s="140">
+      <c r="B82" s="118">
         <f>Архив!A74</f>
         <v>41</v>
       </c>
-      <c r="C82" s="126">
+      <c r="C82" s="119">
         <f>Архив!G74</f>
         <v>28</v>
       </c>
-      <c r="D82" s="127" t="str">
+      <c r="D82" s="120" t="str">
         <f>Архив!B74</f>
         <v>Чеченко Е.Н.</v>
       </c>
@@ -19489,19 +19489,19 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="S82" s="122">
+      <c r="S82" s="121">
         <f>ROUND(SUM(P82:R83),2)</f>
         <v>2190.08</v>
       </c>
-      <c r="T82" s="122">
+      <c r="T82" s="121">
         <f>Архив!E74</f>
         <v>-2420.1599999999958</v>
       </c>
-      <c r="U82" s="122">
+      <c r="U82" s="121">
         <f>Архив!F74</f>
         <v>4000</v>
       </c>
-      <c r="V82" s="122">
+      <c r="V82" s="121">
         <f>SUM(S82:T83)-U82</f>
         <v>-4230.0799999999963</v>
       </c>
@@ -19510,11 +19510,11 @@
     </row>
     <row r="83" spans="1:24" ht="9.75" customHeight="1">
       <c r="A83" s="2"/>
-      <c r="B83" s="140">
+      <c r="B83" s="118">
         <v>39</v>
       </c>
-      <c r="C83" s="126"/>
-      <c r="D83" s="127" t="str">
+      <c r="C83" s="119"/>
+      <c r="D83" s="120" t="str">
         <f>D82</f>
         <v>Чеченко Е.Н.</v>
       </c>
@@ -19570,24 +19570,24 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="S83" s="122"/>
-      <c r="T83" s="122"/>
-      <c r="U83" s="122"/>
-      <c r="V83" s="122"/>
+      <c r="S83" s="121"/>
+      <c r="T83" s="121"/>
+      <c r="U83" s="121"/>
+      <c r="V83" s="121"/>
       <c r="W83" s="6"/>
       <c r="X83" s="6"/>
     </row>
     <row r="84" spans="1:24" ht="9.75" customHeight="1">
       <c r="A84" s="2"/>
-      <c r="B84" s="140">
+      <c r="B84" s="118">
         <f>Архив!A76</f>
         <v>42</v>
       </c>
-      <c r="C84" s="126">
+      <c r="C84" s="119">
         <f>Архив!G76</f>
         <v>16</v>
       </c>
-      <c r="D84" s="127" t="str">
+      <c r="D84" s="120" t="str">
         <f>Архив!B76</f>
         <v>Чихранов А.Д.</v>
       </c>
@@ -19643,19 +19643,19 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S84" s="122">
+      <c r="S84" s="121">
         <f>ROUND(SUM(P84:R85),2)</f>
         <v>916.41</v>
       </c>
-      <c r="T84" s="122">
+      <c r="T84" s="121">
         <f>Архив!E76</f>
         <v>2148.75</v>
       </c>
-      <c r="U84" s="122">
+      <c r="U84" s="121">
         <f>Архив!F76</f>
         <v>2200</v>
       </c>
-      <c r="V84" s="122">
+      <c r="V84" s="121">
         <f>SUM(S84:T85)-U84</f>
         <v>865.15999999999985</v>
       </c>
@@ -19664,11 +19664,11 @@
     </row>
     <row r="85" spans="1:24" ht="9.75" customHeight="1">
       <c r="A85" s="2"/>
-      <c r="B85" s="140">
+      <c r="B85" s="118">
         <v>40</v>
       </c>
-      <c r="C85" s="126"/>
-      <c r="D85" s="127" t="str">
+      <c r="C85" s="119"/>
+      <c r="D85" s="120" t="str">
         <f>D84</f>
         <v>Чихранов А.Д.</v>
       </c>
@@ -19724,24 +19724,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S85" s="122"/>
-      <c r="T85" s="122"/>
-      <c r="U85" s="122"/>
-      <c r="V85" s="122"/>
+      <c r="S85" s="121"/>
+      <c r="T85" s="121"/>
+      <c r="U85" s="121"/>
+      <c r="V85" s="121"/>
       <c r="W85" s="6"/>
       <c r="X85" s="6"/>
     </row>
     <row r="86" spans="1:24" ht="9.75" customHeight="1">
       <c r="A86" s="2"/>
-      <c r="B86" s="140">
+      <c r="B86" s="118">
         <f>Архив!A78</f>
         <v>43</v>
       </c>
-      <c r="C86" s="126">
+      <c r="C86" s="119">
         <f>Архив!G78</f>
         <v>45</v>
       </c>
-      <c r="D86" s="127" t="str">
+      <c r="D86" s="120" t="str">
         <f>Архив!B78</f>
         <v>Шавриева А.В.</v>
       </c>
@@ -19797,19 +19797,19 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S86" s="122">
+      <c r="S86" s="121">
         <f>ROUND(SUM(P86:R87),2)</f>
         <v>1619.73</v>
       </c>
-      <c r="T86" s="122">
+      <c r="T86" s="121">
         <f>Архив!E78</f>
         <v>2226.6600000000003</v>
       </c>
-      <c r="U86" s="122">
+      <c r="U86" s="121">
         <f>Архив!F78</f>
         <v>2226.66</v>
       </c>
-      <c r="V86" s="122">
+      <c r="V86" s="121">
         <f>SUM(S86:T87)-U86</f>
         <v>1619.7300000000005</v>
       </c>
@@ -19818,11 +19818,11 @@
     </row>
     <row r="87" spans="1:24" ht="9.75" customHeight="1">
       <c r="A87" s="2"/>
-      <c r="B87" s="140">
+      <c r="B87" s="118">
         <v>41</v>
       </c>
-      <c r="C87" s="126"/>
-      <c r="D87" s="127" t="str">
+      <c r="C87" s="119"/>
+      <c r="D87" s="120" t="str">
         <f>D86</f>
         <v>Шавриева А.В.</v>
       </c>
@@ -19878,24 +19878,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S87" s="122"/>
-      <c r="T87" s="122"/>
-      <c r="U87" s="122"/>
-      <c r="V87" s="122"/>
+      <c r="S87" s="121"/>
+      <c r="T87" s="121"/>
+      <c r="U87" s="121"/>
+      <c r="V87" s="121"/>
       <c r="W87" s="6"/>
       <c r="X87" s="6"/>
     </row>
     <row r="88" spans="1:24" ht="9.75" customHeight="1">
       <c r="A88" s="2"/>
-      <c r="B88" s="140">
+      <c r="B88" s="118">
         <f>Архив!A80</f>
         <v>44</v>
       </c>
-      <c r="C88" s="126">
+      <c r="C88" s="119">
         <f>Архив!G80</f>
         <v>14</v>
       </c>
-      <c r="D88" s="127" t="str">
+      <c r="D88" s="120" t="str">
         <f>Архив!B80</f>
         <v>Шепелин В.С.</v>
       </c>
@@ -19951,19 +19951,19 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S88" s="122">
+      <c r="S88" s="121">
         <f>ROUND(SUM(P88:R89),2)</f>
         <v>1089.06</v>
       </c>
-      <c r="T88" s="122">
+      <c r="T88" s="121">
         <f>Архив!E80</f>
         <v>1035.9599999999994</v>
       </c>
-      <c r="U88" s="122">
+      <c r="U88" s="121">
         <f>Архив!F80</f>
         <v>1035.96</v>
       </c>
-      <c r="V88" s="122">
+      <c r="V88" s="121">
         <f>SUM(S88:T89)-U88</f>
         <v>1089.0599999999995</v>
       </c>
@@ -19972,11 +19972,11 @@
     </row>
     <row r="89" spans="1:24" ht="9.75" customHeight="1">
       <c r="A89" s="2"/>
-      <c r="B89" s="140">
+      <c r="B89" s="118">
         <v>42</v>
       </c>
-      <c r="C89" s="126"/>
-      <c r="D89" s="127" t="str">
+      <c r="C89" s="119"/>
+      <c r="D89" s="120" t="str">
         <f>D88</f>
         <v>Шепелин В.С.</v>
       </c>
@@ -20032,24 +20032,24 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="S89" s="122"/>
-      <c r="T89" s="122"/>
-      <c r="U89" s="122"/>
-      <c r="V89" s="122"/>
+      <c r="S89" s="121"/>
+      <c r="T89" s="121"/>
+      <c r="U89" s="121"/>
+      <c r="V89" s="121"/>
       <c r="W89" s="6"/>
       <c r="X89" s="6"/>
     </row>
     <row r="90" spans="1:24" ht="9.75" customHeight="1">
       <c r="A90" s="2"/>
-      <c r="B90" s="140">
+      <c r="B90" s="118">
         <f>Архив!A82</f>
         <v>45</v>
       </c>
-      <c r="C90" s="126">
+      <c r="C90" s="119">
         <f>Архив!G82</f>
         <v>59</v>
       </c>
-      <c r="D90" s="127" t="str">
+      <c r="D90" s="120" t="str">
         <f>Архив!B82</f>
         <v>Штетальный В.Г.</v>
       </c>
@@ -20105,19 +20105,19 @@
         <f>IF(L90&lt;0,0,L90*O90)</f>
         <v>0</v>
       </c>
-      <c r="S90" s="122">
+      <c r="S90" s="121">
         <f>ROUND(SUM(P90:R91),2)</f>
         <v>2765.56</v>
       </c>
-      <c r="T90" s="122">
+      <c r="T90" s="121">
         <f>Архив!E82</f>
         <v>2553.3799999999992</v>
       </c>
-      <c r="U90" s="122">
+      <c r="U90" s="121">
         <f>Архив!F82</f>
         <v>2555</v>
       </c>
-      <c r="V90" s="122">
+      <c r="V90" s="121">
         <f>SUM(S90:T91)-U90</f>
         <v>2763.9399999999987</v>
       </c>
@@ -20126,11 +20126,11 @@
     </row>
     <row r="91" spans="1:24" ht="9.75" customHeight="1">
       <c r="A91" s="2"/>
-      <c r="B91" s="140">
+      <c r="B91" s="118">
         <v>43</v>
       </c>
-      <c r="C91" s="126"/>
-      <c r="D91" s="127" t="str">
+      <c r="C91" s="119"/>
+      <c r="D91" s="120" t="str">
         <f>D90</f>
         <v>Штетальный В.Г.</v>
       </c>
@@ -20186,10 +20186,10 @@
         <f>IF(L91&lt;0,0,L91*O91)</f>
         <v>0</v>
       </c>
-      <c r="S91" s="122"/>
-      <c r="T91" s="122"/>
-      <c r="U91" s="122"/>
-      <c r="V91" s="122"/>
+      <c r="S91" s="121"/>
+      <c r="T91" s="121"/>
+      <c r="U91" s="121"/>
+      <c r="V91" s="121"/>
       <c r="W91" s="6"/>
       <c r="X91" s="6"/>
     </row>
@@ -20255,7 +20255,7 @@
     </row>
     <row r="94" spans="1:24" ht="87.75" customHeight="1">
       <c r="A94" s="7"/>
-      <c r="B94" s="121" t="str">
+      <c r="B94" s="140" t="str">
         <f>Архив!B87</f>
         <v>По решению общего собрания потери в электросети ТСН по итогам года рассчитываются равным образом между потребителями. 
 Согласно приложению к приказу №185-УТ от 09.12.2024 г. Управления по тарифам города Севастополя на электроэнергию для населения и приравненных к нему категорий потребителей СНТ в г. Севастополе:
@@ -20265,25 +20265,25 @@
 - в дифференцированном по двум зонам суток, ночной тариф на электрическую энергию, в I-полугодие/II-полугодие составляет: объем, 
 потребляемый до 150 кВт*ч – 3,13/3,52 руб./кВт*ч; объем от 151 кВт*ч до 600 кВт*ч– 3,74/4,21 руб./кВт*ч; объем более 600 кВт*ч – 6,21/6,99 руб./кВт*ч.</v>
       </c>
-      <c r="C94" s="121"/>
-      <c r="D94" s="121"/>
-      <c r="E94" s="121"/>
-      <c r="F94" s="121"/>
-      <c r="G94" s="121"/>
-      <c r="H94" s="121"/>
-      <c r="I94" s="121"/>
-      <c r="J94" s="121"/>
-      <c r="K94" s="121"/>
-      <c r="L94" s="121"/>
-      <c r="M94" s="121"/>
-      <c r="N94" s="121"/>
-      <c r="O94" s="121"/>
-      <c r="P94" s="121"/>
-      <c r="Q94" s="121"/>
-      <c r="R94" s="121"/>
-      <c r="S94" s="121"/>
-      <c r="T94" s="121"/>
-      <c r="U94" s="121"/>
+      <c r="C94" s="140"/>
+      <c r="D94" s="140"/>
+      <c r="E94" s="140"/>
+      <c r="F94" s="140"/>
+      <c r="G94" s="140"/>
+      <c r="H94" s="140"/>
+      <c r="I94" s="140"/>
+      <c r="J94" s="140"/>
+      <c r="K94" s="140"/>
+      <c r="L94" s="140"/>
+      <c r="M94" s="140"/>
+      <c r="N94" s="140"/>
+      <c r="O94" s="140"/>
+      <c r="P94" s="140"/>
+      <c r="Q94" s="140"/>
+      <c r="R94" s="140"/>
+      <c r="S94" s="140"/>
+      <c r="T94" s="140"/>
+      <c r="U94" s="140"/>
       <c r="V94" s="59"/>
     </row>
     <row r="95" spans="1:24" ht="12.75" customHeight="1">
@@ -20453,6 +20453,252 @@
   </sheetData>
   <autoFilter ref="B9:V94" xr:uid="{36175179-D993-184C-875C-B8BBD17289E0}"/>
   <mergeCells count="270">
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="B94:U94"/>
+    <mergeCell ref="V37:V38"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="V27:V28"/>
+    <mergeCell ref="V29:V30"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="U35:U36"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="T35:T36"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="V33:V34"/>
+    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="T23:T24"/>
+    <mergeCell ref="U23:U24"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="S23:S24"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="V18:V19"/>
+    <mergeCell ref="V21:V22"/>
+    <mergeCell ref="V23:V24"/>
+    <mergeCell ref="V31:V32"/>
+    <mergeCell ref="V35:V36"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T14:T15"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="S31:S32"/>
+    <mergeCell ref="T31:T32"/>
+    <mergeCell ref="U31:U32"/>
+    <mergeCell ref="T21:T22"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="S35:S36"/>
+    <mergeCell ref="S27:S28"/>
+    <mergeCell ref="T27:T28"/>
+    <mergeCell ref="U27:U28"/>
+    <mergeCell ref="U25:U26"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="S12:S13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="S29:S30"/>
+    <mergeCell ref="T29:T30"/>
+    <mergeCell ref="U29:U30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="T18:T19"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="S33:S34"/>
+    <mergeCell ref="T33:T34"/>
+    <mergeCell ref="U33:U34"/>
+    <mergeCell ref="S37:S38"/>
+    <mergeCell ref="T37:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="U44:U45"/>
+    <mergeCell ref="U37:U38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="S39:S40"/>
+    <mergeCell ref="T39:T40"/>
+    <mergeCell ref="U39:U40"/>
+    <mergeCell ref="V47:V48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="S47:S48"/>
+    <mergeCell ref="T47:T48"/>
+    <mergeCell ref="U47:U48"/>
+    <mergeCell ref="V44:V45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="T42:T43"/>
+    <mergeCell ref="U42:U43"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="S90:S91"/>
+    <mergeCell ref="T90:T91"/>
+    <mergeCell ref="U90:U91"/>
+    <mergeCell ref="S49:S50"/>
+    <mergeCell ref="T49:T50"/>
+    <mergeCell ref="U49:U50"/>
+    <mergeCell ref="V49:V50"/>
+    <mergeCell ref="V90:V91"/>
+    <mergeCell ref="T61:T62"/>
+    <mergeCell ref="U61:U62"/>
+    <mergeCell ref="V61:V62"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="S55:S56"/>
+    <mergeCell ref="T55:T56"/>
+    <mergeCell ref="U55:U56"/>
+    <mergeCell ref="V55:V56"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="S51:S52"/>
+    <mergeCell ref="S68:S69"/>
+    <mergeCell ref="T68:T69"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="S57:S58"/>
+    <mergeCell ref="T57:T58"/>
+    <mergeCell ref="U57:U58"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="S61:S62"/>
+    <mergeCell ref="V68:V69"/>
+    <mergeCell ref="T59:T60"/>
+    <mergeCell ref="U59:U60"/>
+    <mergeCell ref="V57:V58"/>
+    <mergeCell ref="V59:V60"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="S64:S65"/>
+    <mergeCell ref="T64:T65"/>
+    <mergeCell ref="U64:U65"/>
+    <mergeCell ref="V64:V65"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="S66:S67"/>
+    <mergeCell ref="T66:T67"/>
+    <mergeCell ref="V66:V67"/>
+    <mergeCell ref="U66:U67"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="S70:S71"/>
+    <mergeCell ref="T70:T71"/>
+    <mergeCell ref="U70:U71"/>
+    <mergeCell ref="V70:V71"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="S72:S73"/>
+    <mergeCell ref="T72:T73"/>
+    <mergeCell ref="S75:S76"/>
+    <mergeCell ref="T75:T76"/>
+    <mergeCell ref="U75:U76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V72:V73"/>
+    <mergeCell ref="U72:U73"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="U68:U69"/>
+    <mergeCell ref="U88:U89"/>
+    <mergeCell ref="V84:V85"/>
+    <mergeCell ref="V79:V80"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="S77:S78"/>
+    <mergeCell ref="T77:T78"/>
+    <mergeCell ref="U77:U78"/>
+    <mergeCell ref="S82:S83"/>
+    <mergeCell ref="T82:T83"/>
+    <mergeCell ref="U82:U83"/>
+    <mergeCell ref="V82:V83"/>
+    <mergeCell ref="V39:V40"/>
+    <mergeCell ref="V88:V89"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="S84:S85"/>
+    <mergeCell ref="T84:T85"/>
+    <mergeCell ref="U84:U85"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="V86:V87"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V42:V43"/>
+    <mergeCell ref="S42:S43"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="S59:S60"/>
+    <mergeCell ref="T51:T52"/>
+    <mergeCell ref="U51:U52"/>
+    <mergeCell ref="V51:V52"/>
+    <mergeCell ref="S88:S89"/>
+    <mergeCell ref="T88:T89"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="S86:S87"/>
+    <mergeCell ref="T86:T87"/>
+    <mergeCell ref="U86:U87"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="S79:S80"/>
+    <mergeCell ref="T79:T80"/>
+    <mergeCell ref="U79:U80"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
     <mergeCell ref="B90:B91"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B75:B76"/>
@@ -20477,252 +20723,6 @@
     <mergeCell ref="B82:B83"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="C79:C80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="S86:S87"/>
-    <mergeCell ref="T86:T87"/>
-    <mergeCell ref="U86:U87"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="S79:S80"/>
-    <mergeCell ref="T79:T80"/>
-    <mergeCell ref="U79:U80"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="V39:V40"/>
-    <mergeCell ref="V88:V89"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="S84:S85"/>
-    <mergeCell ref="T84:T85"/>
-    <mergeCell ref="U84:U85"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="V86:V87"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V42:V43"/>
-    <mergeCell ref="S42:S43"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="S59:S60"/>
-    <mergeCell ref="T51:T52"/>
-    <mergeCell ref="U51:U52"/>
-    <mergeCell ref="V51:V52"/>
-    <mergeCell ref="S88:S89"/>
-    <mergeCell ref="T88:T89"/>
-    <mergeCell ref="U88:U89"/>
-    <mergeCell ref="V84:V85"/>
-    <mergeCell ref="V79:V80"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="S77:S78"/>
-    <mergeCell ref="T77:T78"/>
-    <mergeCell ref="U77:U78"/>
-    <mergeCell ref="S82:S83"/>
-    <mergeCell ref="T82:T83"/>
-    <mergeCell ref="U82:U83"/>
-    <mergeCell ref="V82:V83"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="S70:S71"/>
-    <mergeCell ref="T70:T71"/>
-    <mergeCell ref="U70:U71"/>
-    <mergeCell ref="V70:V71"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="S72:S73"/>
-    <mergeCell ref="T72:T73"/>
-    <mergeCell ref="S75:S76"/>
-    <mergeCell ref="T75:T76"/>
-    <mergeCell ref="U75:U76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V72:V73"/>
-    <mergeCell ref="U72:U73"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="S64:S65"/>
-    <mergeCell ref="T64:T65"/>
-    <mergeCell ref="U64:U65"/>
-    <mergeCell ref="V64:V65"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="S66:S67"/>
-    <mergeCell ref="T66:T67"/>
-    <mergeCell ref="V66:V67"/>
-    <mergeCell ref="U68:U69"/>
-    <mergeCell ref="U66:U67"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="S57:S58"/>
-    <mergeCell ref="T57:T58"/>
-    <mergeCell ref="U57:U58"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="S61:S62"/>
-    <mergeCell ref="V68:V69"/>
-    <mergeCell ref="T59:T60"/>
-    <mergeCell ref="U59:U60"/>
-    <mergeCell ref="V57:V58"/>
-    <mergeCell ref="V59:V60"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="S90:S91"/>
-    <mergeCell ref="T90:T91"/>
-    <mergeCell ref="U90:U91"/>
-    <mergeCell ref="S49:S50"/>
-    <mergeCell ref="T49:T50"/>
-    <mergeCell ref="U49:U50"/>
-    <mergeCell ref="V49:V50"/>
-    <mergeCell ref="V90:V91"/>
-    <mergeCell ref="T61:T62"/>
-    <mergeCell ref="U61:U62"/>
-    <mergeCell ref="V61:V62"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="S55:S56"/>
-    <mergeCell ref="T55:T56"/>
-    <mergeCell ref="U55:U56"/>
-    <mergeCell ref="V55:V56"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="S51:S52"/>
-    <mergeCell ref="S68:S69"/>
-    <mergeCell ref="T68:T69"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="S39:S40"/>
-    <mergeCell ref="T39:T40"/>
-    <mergeCell ref="U39:U40"/>
-    <mergeCell ref="V47:V48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="S47:S48"/>
-    <mergeCell ref="T47:T48"/>
-    <mergeCell ref="U47:U48"/>
-    <mergeCell ref="V44:V45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="T42:T43"/>
-    <mergeCell ref="U42:U43"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="S33:S34"/>
-    <mergeCell ref="T33:T34"/>
-    <mergeCell ref="U33:U34"/>
-    <mergeCell ref="S37:S38"/>
-    <mergeCell ref="T37:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="U44:U45"/>
-    <mergeCell ref="U37:U38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="S29:S30"/>
-    <mergeCell ref="T29:T30"/>
-    <mergeCell ref="U29:U30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="S18:S19"/>
-    <mergeCell ref="T18:T19"/>
-    <mergeCell ref="S16:S17"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="S12:S13"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="V18:V19"/>
-    <mergeCell ref="V21:V22"/>
-    <mergeCell ref="V23:V24"/>
-    <mergeCell ref="V31:V32"/>
-    <mergeCell ref="V35:V36"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T14:T15"/>
-    <mergeCell ref="S14:S15"/>
-    <mergeCell ref="S31:S32"/>
-    <mergeCell ref="T31:T32"/>
-    <mergeCell ref="U31:U32"/>
-    <mergeCell ref="T21:T22"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="S21:S22"/>
-    <mergeCell ref="S35:S36"/>
-    <mergeCell ref="S27:S28"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="U27:U28"/>
-    <mergeCell ref="U25:U26"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="S25:S26"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="B94:U94"/>
-    <mergeCell ref="V37:V38"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="V27:V28"/>
-    <mergeCell ref="V29:V30"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="U35:U36"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="T35:T36"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="V33:V34"/>
-    <mergeCell ref="T12:T13"/>
-    <mergeCell ref="T23:T24"/>
-    <mergeCell ref="U23:U24"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="S23:S24"/>
-    <mergeCell ref="U21:U22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.39370078740157499" right="0.196850393700787" top="0.196850393700787" bottom="0.196850393700787" header="0.511811023622047" footer="0.511811023622047"/>
@@ -20782,11 +20782,11 @@
       <c r="Q1" s="110"/>
       <c r="R1" s="110"/>
       <c r="S1" s="111"/>
-      <c r="T1" s="120" t="d">
+      <c r="T1" s="139" t="d">
         <f>Архив!B1</f>
         <v>2025-10-01</v>
       </c>
-      <c r="U1" s="120"/>
+      <c r="U1" s="139"/>
       <c r="V1" s="107"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1">
@@ -20925,48 +20925,48 @@
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="21.75" customHeight="1">
       <c r="A7" s="20"/>
-      <c r="B7" s="145" t="str">
+      <c r="B7" s="141" t="str">
         <f>Calc!B7</f>
         <v>г. Севастополь,
 ТСН "ЖСТИЗ "СТОЛЕТОВСКИЙ"</v>
       </c>
-      <c r="C7" s="146"/>
-      <c r="D7" s="147"/>
-      <c r="E7" s="131" t="str">
+      <c r="C7" s="142"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="130" t="str">
         <f>Calc!F7</f>
         <v>Показания по прибору учета электроэнергии</v>
       </c>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="131" t="s">
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="132"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="131" t="s">
+      <c r="J7" s="131"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="132"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="131" t="s">
+      <c r="M7" s="131"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="132"/>
-      <c r="Q7" s="133"/>
-      <c r="R7" s="123" t="str">
+      <c r="P7" s="131"/>
+      <c r="Q7" s="132"/>
+      <c r="R7" s="137" t="str">
         <f>Calc!S7</f>
         <v>Сумма, руб.</v>
       </c>
-      <c r="S7" s="135" t="str">
+      <c r="S7" s="133" t="str">
         <f>Calc!T7</f>
         <v>Долг / Переплата "-", руб.</v>
       </c>
-      <c r="T7" s="123" t="str">
+      <c r="T7" s="137" t="str">
         <f>Calc!U7</f>
         <v>Учтена оплата, руб.</v>
       </c>
-      <c r="U7" s="123" t="str">
+      <c r="U7" s="137" t="str">
         <f>Calc!V7</f>
         <v>К оплате, руб.</v>
       </c>
@@ -21039,20 +21039,20 @@
         <f>Calc!R8</f>
         <v>Блок 3</v>
       </c>
-      <c r="R8" s="124"/>
-      <c r="S8" s="136"/>
-      <c r="T8" s="124"/>
-      <c r="U8" s="124"/>
+      <c r="R8" s="138"/>
+      <c r="S8" s="134"/>
+      <c r="T8" s="138"/>
+      <c r="U8" s="138"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
     </row>
     <row r="9" spans="1:23" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A9" s="21"/>
-      <c r="B9" s="126">
+      <c r="B9" s="119">
         <f>Calc!C10</f>
         <v>21</v>
       </c>
-      <c r="C9" s="137" t="str">
+      <c r="C9" s="135" t="str">
         <f>Calc!D10</f>
         <v>Гаценко Н.Г.</v>
       </c>
@@ -21112,19 +21112,19 @@
         <f>Calc!R10</f>
         <v>0</v>
       </c>
-      <c r="R9" s="122">
+      <c r="R9" s="121">
         <f>Calc!S10</f>
         <v>30.59</v>
       </c>
-      <c r="S9" s="122">
+      <c r="S9" s="121">
         <f>Calc!T10</f>
         <v>-282.56999999999988</v>
       </c>
-      <c r="T9" s="122">
+      <c r="T9" s="121">
         <f>Calc!U10</f>
         <v>500</v>
       </c>
-      <c r="U9" s="122">
+      <c r="U9" s="121">
         <f>Calc!V10</f>
         <v>-751.9799999999999</v>
       </c>
@@ -21133,8 +21133,8 @@
     </row>
     <row r="10" spans="1:23" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A10" s="21"/>
-      <c r="B10" s="126"/>
-      <c r="C10" s="138"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="136"/>
       <c r="D10" s="12" t="str">
         <f>Calc!E11</f>
         <v>Ночь (Т2)</v>
@@ -21191,10 +21191,10 @@
         <f>Calc!R11</f>
         <v>0</v>
       </c>
-      <c r="R10" s="122"/>
-      <c r="S10" s="122"/>
-      <c r="T10" s="122"/>
-      <c r="U10" s="122"/>
+      <c r="R10" s="121"/>
+      <c r="S10" s="121"/>
+      <c r="T10" s="121"/>
+      <c r="U10" s="121"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
     </row>
@@ -21224,7 +21224,7 @@
     </row>
     <row r="12" spans="1:23" ht="110" customHeight="1">
       <c r="A12" s="20"/>
-      <c r="B12" s="121" t="str">
+      <c r="B12" s="140" t="str">
         <f>Архив!B87</f>
         <v>По решению общего собрания потери в электросети ТСН по итогам года рассчитываются равным образом между потребителями. 
 Согласно приложению к приказу №185-УТ от 09.12.2024 г. Управления по тарифам города Севастополя на электроэнергию для населения и приравненных к нему категорий потребителей СНТ в г. Севастополе:
@@ -21234,25 +21234,25 @@
 - в дифференцированном по двум зонам суток, ночной тариф на электрическую энергию, в I-полугодие/II-полугодие составляет: объем, 
 потребляемый до 150 кВт*ч – 3,13/3,52 руб./кВт*ч; объем от 151 кВт*ч до 600 кВт*ч– 3,74/4,21 руб./кВт*ч; объем более 600 кВт*ч – 6,21/6,99 руб./кВт*ч.</v>
       </c>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="121"/>
-      <c r="I12" s="121"/>
-      <c r="J12" s="121"/>
-      <c r="K12" s="121"/>
-      <c r="L12" s="121"/>
-      <c r="M12" s="121"/>
-      <c r="N12" s="121"/>
-      <c r="O12" s="121"/>
-      <c r="P12" s="121"/>
-      <c r="Q12" s="121"/>
-      <c r="R12" s="121"/>
-      <c r="S12" s="121"/>
-      <c r="T12" s="121"/>
-      <c r="U12" s="121"/>
+      <c r="C12" s="140"/>
+      <c r="D12" s="140"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="140"/>
+      <c r="J12" s="140"/>
+      <c r="K12" s="140"/>
+      <c r="L12" s="140"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="140"/>
+      <c r="O12" s="140"/>
+      <c r="P12" s="140"/>
+      <c r="Q12" s="140"/>
+      <c r="R12" s="140"/>
+      <c r="S12" s="140"/>
+      <c r="T12" s="140"/>
+      <c r="U12" s="140"/>
       <c r="V12" s="20"/>
     </row>
     <row r="13" spans="1:23">
@@ -21347,11 +21347,11 @@
       <c r="Q16" s="110"/>
       <c r="R16" s="110"/>
       <c r="S16" s="111"/>
-      <c r="T16" s="120" t="d">
+      <c r="T16" s="139" t="d">
         <f>Архив!B1</f>
         <v>2025-10-01</v>
       </c>
-      <c r="U16" s="120"/>
+      <c r="U16" s="139"/>
       <c r="V16" s="107"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1">
@@ -21490,48 +21490,48 @@
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="21.75" customHeight="1">
       <c r="A22" s="20"/>
-      <c r="B22" s="145" t="str">
+      <c r="B22" s="141" t="str">
         <f>Calc!B7</f>
         <v>г. Севастополь,
 ТСН "ЖСТИЗ "СТОЛЕТОВСКИЙ"</v>
       </c>
-      <c r="C22" s="146"/>
-      <c r="D22" s="147"/>
-      <c r="E22" s="131" t="str">
+      <c r="C22" s="142"/>
+      <c r="D22" s="143"/>
+      <c r="E22" s="130" t="str">
         <f>Calc!F7</f>
         <v>Показания по прибору учета электроэнергии</v>
       </c>
-      <c r="F22" s="132"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="131" t="s">
+      <c r="F22" s="131"/>
+      <c r="G22" s="131"/>
+      <c r="H22" s="132"/>
+      <c r="I22" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="132"/>
-      <c r="K22" s="133"/>
-      <c r="L22" s="131" t="s">
+      <c r="J22" s="131"/>
+      <c r="K22" s="132"/>
+      <c r="L22" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="M22" s="132"/>
-      <c r="N22" s="133"/>
-      <c r="O22" s="131" t="s">
+      <c r="M22" s="131"/>
+      <c r="N22" s="132"/>
+      <c r="O22" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="P22" s="132"/>
-      <c r="Q22" s="133"/>
-      <c r="R22" s="123" t="str">
+      <c r="P22" s="131"/>
+      <c r="Q22" s="132"/>
+      <c r="R22" s="137" t="str">
         <f>Calc!S7</f>
         <v>Сумма, руб.</v>
       </c>
-      <c r="S22" s="123" t="str">
+      <c r="S22" s="137" t="str">
         <f>Calc!T7</f>
         <v>Долг / Переплата "-", руб.</v>
       </c>
-      <c r="T22" s="123" t="str">
+      <c r="T22" s="137" t="str">
         <f>Calc!U7</f>
         <v>Учтена оплата, руб.</v>
       </c>
-      <c r="U22" s="123" t="str">
+      <c r="U22" s="137" t="str">
         <f>Calc!V7</f>
         <v>К оплате, руб.</v>
       </c>
@@ -21604,20 +21604,20 @@
         <f>Calc!R8</f>
         <v>Блок 3</v>
       </c>
-      <c r="R23" s="124"/>
-      <c r="S23" s="124"/>
-      <c r="T23" s="124"/>
-      <c r="U23" s="124"/>
+      <c r="R23" s="138"/>
+      <c r="S23" s="138"/>
+      <c r="T23" s="138"/>
+      <c r="U23" s="138"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
     </row>
     <row r="24" spans="1:23" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A24" s="21"/>
-      <c r="B24" s="126">
+      <c r="B24" s="119">
         <f>Calc!C12</f>
         <v>54</v>
       </c>
-      <c r="C24" s="137" t="str">
+      <c r="C24" s="135" t="str">
         <f>Calc!D12</f>
         <v>Дикарев А.А.</v>
       </c>
@@ -21677,19 +21677,19 @@
         <f>Calc!R12</f>
         <v>0</v>
       </c>
-      <c r="R24" s="122">
+      <c r="R24" s="121">
         <f>Calc!S12</f>
         <v>0</v>
       </c>
-      <c r="S24" s="122">
+      <c r="S24" s="121">
         <f>Calc!T12</f>
         <v>0</v>
       </c>
-      <c r="T24" s="122">
+      <c r="T24" s="121">
         <f>Calc!U12</f>
         <v>0</v>
       </c>
-      <c r="U24" s="122">
+      <c r="U24" s="121">
         <f>Calc!V12</f>
         <v>0</v>
       </c>
@@ -21698,8 +21698,8 @@
     </row>
     <row r="25" spans="1:23" s="23" customFormat="1" ht="9.75" customHeight="1">
       <c r="A25" s="21"/>
-      <c r="B25" s="126"/>
-      <c r="C25" s="138"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="136"/>
       <c r="D25" s="12" t="str">
         <f>Calc!E13</f>
         <v>Ночь (Т2)</v>
@@ -21756,10 +21756,10 @@
         <f>Calc!R13</f>
         <v>0</v>
       </c>
-      <c r="R25" s="122"/>
-      <c r="S25" s="122"/>
-      <c r="T25" s="122"/>
-      <c r="U25" s="122"/>
+      <c r="R25" s="121"/>
+      <c r="S25" s="121"/>
+      <c r="T25" s="121"/>
+      <c r="U25" s="121"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
     </row>
@@ -21789,7 +21789,7 @@
     </row>
     <row r="27" spans="1:23" ht="110" customHeight="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="121" t="str">
+      <c r="B27" s="140" t="str">
         <f>Архив!B87</f>
         <v>По решению общего собрания потери в электросети ТСН по итогам года рассчитываются равным образом между потребителями. 
 Согласно приложению к приказу №185-УТ от 09.12.2024 г. Управления по тарифам города Севастополя на электроэнергию для населения и приравненных к нему категорий потребителей СНТ в г. Севастополе:
@@ -21799,25 +21799,25 @@
 - в дифференцированном по двум зонам суток, ночной тариф на электрическую энергию, в I-полугодие/II-полугодие составляет: объем, 
 потребляемый до 150 кВт*ч – 3,13/3,52 руб./кВт*ч; объем от 151 кВт*ч до 600 кВт*ч– 3,74/4,21 руб./кВт*ч; объем более 600 кВт*ч – 6,21/6,99 руб./кВт*ч.</v>
       </c>
-      <c r="C27" s="121"/>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="121"/>
-      <c r="J27" s="121"/>
-      <c r="K27" s="121"/>
-      <c r="L27" s="121"/>
-      <c r="M27" s="121"/>
-      <c r="N27" s="121"/>
-      <c r="O27" s="121"/>
-      <c r="P27" s="121"/>
-      <c r="Q27" s="121"/>
-      <c r="R27" s="121"/>
-      <c r="S27" s="121"/>
-      <c r="T27" s="121"/>
-      <c r="U27" s="121"/>
+      <c r="C27" s="140"/>
+      <c r="D27" s="140"/>
+      <c r="E27" s="140"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="140"/>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="140"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="140"/>
+      <c r="N27" s="140"/>
+      <c r="O27" s="140"/>
+      <c r="P27" s="140"/>
+      <c r="Q27" s="140"/>
+      <c r="R27" s="140"/>
+      <c r="S27" s="140"/>
+      <c r="T27" s="140"/>
+      <c r="U27" s="140"/>
       <c r="V27" s="20"/>
     </row>
     <row r="28" spans="1:23" ht="15" customHeight="1">
@@ -21888,10 +21888,10 @@
       <c r="Q30" s="110"/>
       <c r="R30" s="110"/>
       <c r="S30" s="111"/>
-      <c r="T30" s="120" t="d">
+      <c r="T30" s="139" t="d">
         <v>2025-02-01</v>
       </c>
-      <c r="U30" s="120"/>
+      <c r="U30" s="139"/>
       <c r="V30" s="107"/>
       <c r="W30" s="1"/>
     </row>
@@ -22028,42 +22028,42 @@
     </row>
     <row r="36" spans="1:23" ht="9.75" customHeight="1">
       <c r="A36" s="20"/>
-      <c r="B36" s="145" t="s">
+      <c r="B36" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="146"/>
-      <c r="D36" s="147"/>
-      <c r="E36" s="131" t="s">
+      <c r="C36" s="142"/>
+      <c r="D36" s="143"/>
+      <c r="E36" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="132"/>
-      <c r="G36" s="132"/>
-      <c r="H36" s="133"/>
-      <c r="I36" s="131" t="s">
+      <c r="F36" s="131"/>
+      <c r="G36" s="131"/>
+      <c r="H36" s="132"/>
+      <c r="I36" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="J36" s="132"/>
-      <c r="K36" s="133"/>
-      <c r="L36" s="131" t="s">
+      <c r="J36" s="131"/>
+      <c r="K36" s="132"/>
+      <c r="L36" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="M36" s="132"/>
-      <c r="N36" s="133"/>
-      <c r="O36" s="131" t="s">
+      <c r="M36" s="131"/>
+      <c r="N36" s="132"/>
+      <c r="O36" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="P36" s="132"/>
-      <c r="Q36" s="133"/>
-      <c r="R36" s="123" t="s">
+      <c r="P36" s="131"/>
+      <c r="Q36" s="132"/>
+      <c r="R36" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="S36" s="123" t="s">
+      <c r="S36" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="T36" s="123" t="s">
+      <c r="T36" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="U36" s="123" t="s">
+      <c r="U36" s="137" t="s">
         <v>11</v>
       </c>
       <c r="V36" s="20"/>
@@ -22119,20 +22119,20 @@
       <c r="Q37" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="R37" s="124"/>
-      <c r="S37" s="124"/>
-      <c r="T37" s="124"/>
-      <c r="U37" s="124"/>
+      <c r="R37" s="138"/>
+      <c r="S37" s="138"/>
+      <c r="T37" s="138"/>
+      <c r="U37" s="138"/>
       <c r="V37" s="6"/>
       <c r="W37" s="6"/>
     </row>
     <row r="38" spans="1:23">
       <c r="A38" s="21"/>
-      <c r="B38" s="141">
+      <c r="B38" s="146">
         <f>Calc!C14</f>
         <v>51</v>
       </c>
-      <c r="C38" s="141" t="str">
+      <c r="C38" s="146" t="str">
         <f>Calc!D14</f>
         <v>Дмитриев А.В.</v>
       </c>
@@ -22192,19 +22192,19 @@
         <f>Calc!R14</f>
         <v>0</v>
       </c>
-      <c r="R38" s="143">
+      <c r="R38" s="144">
         <f>Calc!S14</f>
         <v>2184.7600000000002</v>
       </c>
-      <c r="S38" s="143">
+      <c r="S38" s="144">
         <f>Calc!T14</f>
         <v>8160.23</v>
       </c>
-      <c r="T38" s="143">
+      <c r="T38" s="144">
         <f>Calc!U14</f>
         <v>0</v>
       </c>
-      <c r="U38" s="143">
+      <c r="U38" s="144">
         <f>Calc!V14</f>
         <v>10344.99</v>
       </c>
@@ -22213,8 +22213,8 @@
     </row>
     <row r="39" spans="1:23">
       <c r="A39" s="21"/>
-      <c r="B39" s="142"/>
-      <c r="C39" s="142"/>
+      <c r="B39" s="147"/>
+      <c r="C39" s="147"/>
       <c r="D39" s="12" t="str">
         <f>Calc!E15</f>
         <v>Ночь (Т2)</v>
@@ -22271,10 +22271,10 @@
         <f>Calc!R15</f>
         <v>0</v>
       </c>
-      <c r="R39" s="144"/>
-      <c r="S39" s="144"/>
-      <c r="T39" s="144"/>
-      <c r="U39" s="144"/>
+      <c r="R39" s="145"/>
+      <c r="S39" s="145"/>
+      <c r="T39" s="145"/>
+      <c r="U39" s="145"/>
       <c r="V39" s="6"/>
       <c r="W39" s="6"/>
     </row>
@@ -22304,28 +22304,28 @@
     </row>
     <row r="41" spans="1:23" ht="92.75" customHeight="1">
       <c r="A41" s="20"/>
-      <c r="B41" s="121" t="s">
+      <c r="B41" s="140" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="121"/>
-      <c r="D41" s="121"/>
-      <c r="E41" s="121"/>
-      <c r="F41" s="121"/>
-      <c r="G41" s="121"/>
-      <c r="H41" s="121"/>
-      <c r="I41" s="121"/>
-      <c r="J41" s="121"/>
-      <c r="K41" s="121"/>
-      <c r="L41" s="121"/>
-      <c r="M41" s="121"/>
-      <c r="N41" s="121"/>
-      <c r="O41" s="121"/>
-      <c r="P41" s="121"/>
-      <c r="Q41" s="121"/>
-      <c r="R41" s="121"/>
-      <c r="S41" s="121"/>
-      <c r="T41" s="121"/>
-      <c r="U41" s="121"/>
+      <c r="C41" s="140"/>
+      <c r="D41" s="140"/>
+      <c r="E41" s="140"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="140"/>
+      <c r="I41" s="140"/>
+      <c r="J41" s="140"/>
+      <c r="K41" s="140"/>
+      <c r="L41" s="140"/>
+      <c r="M41" s="140"/>
+      <c r="N41" s="140"/>
+      <c r="O41" s="140"/>
+      <c r="P41" s="140"/>
+      <c r="Q41" s="140"/>
+      <c r="R41" s="140"/>
+      <c r="S41" s="140"/>
+      <c r="T41" s="140"/>
+      <c r="U41" s="140"/>
       <c r="V41" s="20"/>
     </row>
     <row r="42" spans="1:23">
@@ -22362,10 +22362,10 @@
       <c r="Q45" s="110"/>
       <c r="R45" s="110"/>
       <c r="S45" s="111"/>
-      <c r="T45" s="120" t="d">
+      <c r="T45" s="139" t="d">
         <v>2025-02-01</v>
       </c>
-      <c r="U45" s="120"/>
+      <c r="U45" s="139"/>
       <c r="V45" s="107"/>
       <c r="W45" s="1"/>
     </row>
@@ -22502,42 +22502,42 @@
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="20"/>
-      <c r="B51" s="145" t="s">
+      <c r="B51" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="146"/>
-      <c r="D51" s="147"/>
-      <c r="E51" s="131" t="s">
+      <c r="C51" s="142"/>
+      <c r="D51" s="143"/>
+      <c r="E51" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="F51" s="132"/>
-      <c r="G51" s="132"/>
-      <c r="H51" s="133"/>
-      <c r="I51" s="131" t="s">
+      <c r="F51" s="131"/>
+      <c r="G51" s="131"/>
+      <c r="H51" s="132"/>
+      <c r="I51" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="J51" s="132"/>
-      <c r="K51" s="133"/>
-      <c r="L51" s="131" t="s">
+      <c r="J51" s="131"/>
+      <c r="K51" s="132"/>
+      <c r="L51" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="M51" s="132"/>
-      <c r="N51" s="133"/>
-      <c r="O51" s="131" t="s">
+      <c r="M51" s="131"/>
+      <c r="N51" s="132"/>
+      <c r="O51" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="P51" s="132"/>
-      <c r="Q51" s="133"/>
-      <c r="R51" s="123" t="s">
+      <c r="P51" s="131"/>
+      <c r="Q51" s="132"/>
+      <c r="R51" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="S51" s="123" t="s">
+      <c r="S51" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="T51" s="123" t="s">
+      <c r="T51" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="U51" s="123" t="s">
+      <c r="U51" s="137" t="s">
         <v>11</v>
       </c>
       <c r="V51" s="20"/>
@@ -22593,20 +22593,20 @@
       <c r="Q52" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="R52" s="124"/>
-      <c r="S52" s="124"/>
-      <c r="T52" s="124"/>
-      <c r="U52" s="124"/>
+      <c r="R52" s="138"/>
+      <c r="S52" s="138"/>
+      <c r="T52" s="138"/>
+      <c r="U52" s="138"/>
       <c r="V52" s="6"/>
       <c r="W52" s="6"/>
     </row>
     <row r="53" spans="1:23">
       <c r="A53" s="21"/>
-      <c r="B53" s="141">
+      <c r="B53" s="146">
         <f>Calc!C16</f>
         <v>35</v>
       </c>
-      <c r="C53" s="141" t="str">
+      <c r="C53" s="146" t="str">
         <f>Calc!D16</f>
         <v>Егоров Е.Ю.</v>
       </c>
@@ -22666,19 +22666,19 @@
         <f>Calc!R16</f>
         <v>0</v>
       </c>
-      <c r="R53" s="143">
+      <c r="R53" s="144">
         <f>Calc!S16</f>
         <v>1212.57</v>
       </c>
-      <c r="S53" s="143">
+      <c r="S53" s="144">
         <f>Calc!T16</f>
         <v>2391.64</v>
       </c>
-      <c r="T53" s="143">
+      <c r="T53" s="144">
         <f>Calc!U16</f>
         <v>0</v>
       </c>
-      <c r="U53" s="143">
+      <c r="U53" s="144">
         <f>Calc!V16</f>
         <v>3604.21</v>
       </c>
@@ -22687,8 +22687,8 @@
     </row>
     <row r="54" spans="1:23">
       <c r="A54" s="21"/>
-      <c r="B54" s="142"/>
-      <c r="C54" s="142"/>
+      <c r="B54" s="147"/>
+      <c r="C54" s="147"/>
       <c r="D54" s="12" t="str">
         <f>Calc!E17</f>
         <v>Ночь (Т2)</v>
@@ -22745,10 +22745,10 @@
         <f>Calc!R17</f>
         <v>0</v>
       </c>
-      <c r="R54" s="144"/>
-      <c r="S54" s="144"/>
-      <c r="T54" s="144"/>
-      <c r="U54" s="144"/>
+      <c r="R54" s="145"/>
+      <c r="S54" s="145"/>
+      <c r="T54" s="145"/>
+      <c r="U54" s="145"/>
       <c r="V54" s="6"/>
       <c r="W54" s="6"/>
     </row>
@@ -22778,28 +22778,28 @@
     </row>
     <row r="56" spans="1:23" ht="78.5" customHeight="1">
       <c r="A56" s="20"/>
-      <c r="B56" s="121" t="s">
+      <c r="B56" s="140" t="s">
         <v>105</v>
       </c>
-      <c r="C56" s="121"/>
-      <c r="D56" s="121"/>
-      <c r="E56" s="121"/>
-      <c r="F56" s="121"/>
-      <c r="G56" s="121"/>
-      <c r="H56" s="121"/>
-      <c r="I56" s="121"/>
-      <c r="J56" s="121"/>
-      <c r="K56" s="121"/>
-      <c r="L56" s="121"/>
-      <c r="M56" s="121"/>
-      <c r="N56" s="121"/>
-      <c r="O56" s="121"/>
-      <c r="P56" s="121"/>
-      <c r="Q56" s="121"/>
-      <c r="R56" s="121"/>
-      <c r="S56" s="121"/>
-      <c r="T56" s="121"/>
-      <c r="U56" s="121"/>
+      <c r="C56" s="140"/>
+      <c r="D56" s="140"/>
+      <c r="E56" s="140"/>
+      <c r="F56" s="140"/>
+      <c r="G56" s="140"/>
+      <c r="H56" s="140"/>
+      <c r="I56" s="140"/>
+      <c r="J56" s="140"/>
+      <c r="K56" s="140"/>
+      <c r="L56" s="140"/>
+      <c r="M56" s="140"/>
+      <c r="N56" s="140"/>
+      <c r="O56" s="140"/>
+      <c r="P56" s="140"/>
+      <c r="Q56" s="140"/>
+      <c r="R56" s="140"/>
+      <c r="S56" s="140"/>
+      <c r="T56" s="140"/>
+      <c r="U56" s="140"/>
       <c r="V56" s="20"/>
     </row>
     <row r="57" spans="1:23">
@@ -22812,6 +22812,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="R51:R52"/>
+    <mergeCell ref="S51:S52"/>
+    <mergeCell ref="B41:U41"/>
+    <mergeCell ref="B56:U56"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="R53:R54"/>
+    <mergeCell ref="S53:S54"/>
+    <mergeCell ref="T53:T54"/>
+    <mergeCell ref="U53:U54"/>
+    <mergeCell ref="T45:U45"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="T51:T52"/>
+    <mergeCell ref="U51:U52"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="O51:Q51"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="O36:Q36"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="S36:S37"/>
+    <mergeCell ref="T36:T37"/>
+    <mergeCell ref="U36:U37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="R38:R39"/>
+    <mergeCell ref="S38:S39"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B12:U12"/>
     <mergeCell ref="B27:U27"/>
     <mergeCell ref="S7:S8"/>
     <mergeCell ref="T7:T8"/>
@@ -22828,58 +22880,6 @@
     <mergeCell ref="U22:U23"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B12:U12"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="R36:R37"/>
-    <mergeCell ref="S36:S37"/>
-    <mergeCell ref="T36:T37"/>
-    <mergeCell ref="U36:U37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="R38:R39"/>
-    <mergeCell ref="S38:S39"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="B41:U41"/>
-    <mergeCell ref="B56:U56"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="R53:R54"/>
-    <mergeCell ref="S53:S54"/>
-    <mergeCell ref="T53:T54"/>
-    <mergeCell ref="U53:U54"/>
-    <mergeCell ref="T45:U45"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="T51:T52"/>
-    <mergeCell ref="U51:U52"/>
-    <mergeCell ref="E51:H51"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="O51:Q51"/>
-    <mergeCell ref="R51:R52"/>
-    <mergeCell ref="S51:S52"/>
   </mergeCells>
   <pageMargins left="0.375" right="0.22222222222222221" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="landscape"/>

</xml_diff>